<commit_message>
attempt to switch the "Basic Parts" tab to "Parts and Devices" Also switch all current libraries Finally, add script testing and refactor scripting to allow unit tests to run
</commit_message>
<xml_diff>
--- a/Anderson Promoters/Anderson Promoters.xlsx
+++ b/Anderson Promoters/Anderson Promoters.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakebeal/projects/BioTools/iGEM_distribution/Anderson Promoters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F17CA301-1C94-5349-836D-77F9FB085E19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B83A4FEC-398A-1C42-A0E5-9C827EE872FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="34060" windowHeight="19800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5480" yWindow="1300" windowWidth="34060" windowHeight="19800" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Basic Parts" sheetId="1" r:id="rId1"/>
+    <sheet name="Parts and Devices" sheetId="1" r:id="rId1"/>
     <sheet name="Libraries and Composites" sheetId="2" r:id="rId2"/>
     <sheet name="Ontology Terms" sheetId="3" r:id="rId3"/>
     <sheet name="Organism Terms" sheetId="4" r:id="rId4"/>
@@ -22641,9 +22641,6 @@
     <t>Template Version:</t>
   </si>
   <si>
-    <t>1.0a1</t>
-  </si>
-  <si>
     <t>Anderson Promoters</t>
   </si>
   <si>
@@ -22714,6 +22711,9 @@
   </si>
   <si>
     <t>Anderson Promoters in vector</t>
+  </si>
+  <si>
+    <t>1.0a2</t>
   </si>
 </sst>
 </file>
@@ -23586,7 +23586,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>7516</v>
+        <v>7515</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="4" t="s">
@@ -23600,7 +23600,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7517</v>
+        <v>7516</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -23637,7 +23637,7 @@
     </row>
     <row r="5" spans="1:13" ht="46" customHeight="1">
       <c r="A5" s="48" t="s">
-        <v>7518</v>
+        <v>7517</v>
       </c>
       <c r="B5" s="49"/>
       <c r="C5" s="49"/>
@@ -23889,7 +23889,7 @@
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1">
       <c r="A15" s="47" t="s">
-        <v>7519</v>
+        <v>7518</v>
       </c>
       <c r="B15" s="46" t="s">
         <v>7506</v>
@@ -23901,7 +23901,7 @@
         <v>43</v>
       </c>
       <c r="G15" s="47" t="s">
-        <v>7519</v>
+        <v>7518</v>
       </c>
       <c r="H15" s="18"/>
       <c r="I15" s="18" t="s">
@@ -23953,7 +23953,7 @@
     </row>
     <row r="17" spans="1:13" ht="15.75" customHeight="1">
       <c r="A17" s="41" t="s">
-        <v>7520</v>
+        <v>7519</v>
       </c>
       <c r="B17" s="41" t="s">
         <v>7506</v>
@@ -23965,7 +23965,7 @@
         <v>43</v>
       </c>
       <c r="G17" s="41" t="s">
-        <v>7520</v>
+        <v>7519</v>
       </c>
       <c r="H17" s="18"/>
       <c r="I17" s="18" t="s">
@@ -23985,7 +23985,7 @@
     </row>
     <row r="18" spans="1:13" ht="15.75" customHeight="1">
       <c r="A18" s="41" t="s">
-        <v>7521</v>
+        <v>7520</v>
       </c>
       <c r="B18" s="41" t="s">
         <v>7506</v>
@@ -23997,7 +23997,7 @@
         <v>43</v>
       </c>
       <c r="G18" s="41" t="s">
-        <v>7521</v>
+        <v>7520</v>
       </c>
       <c r="H18" s="18"/>
       <c r="I18" s="18" t="s">
@@ -24017,7 +24017,7 @@
     </row>
     <row r="19" spans="1:13" ht="15.75" customHeight="1">
       <c r="A19" s="41" t="s">
-        <v>7522</v>
+        <v>7521</v>
       </c>
       <c r="B19" s="41" t="s">
         <v>7506</v>
@@ -24029,7 +24029,7 @@
         <v>43</v>
       </c>
       <c r="G19" s="41" t="s">
-        <v>7522</v>
+        <v>7521</v>
       </c>
       <c r="H19" s="18"/>
       <c r="I19" s="18" t="s">
@@ -24049,7 +24049,7 @@
     </row>
     <row r="20" spans="1:13" ht="15.75" customHeight="1">
       <c r="A20" s="41" t="s">
-        <v>7523</v>
+        <v>7522</v>
       </c>
       <c r="B20" s="46" t="s">
         <v>7506</v>
@@ -24061,7 +24061,7 @@
         <v>43</v>
       </c>
       <c r="G20" s="41" t="s">
-        <v>7523</v>
+        <v>7522</v>
       </c>
       <c r="H20" s="18"/>
       <c r="I20" s="18" t="s">
@@ -24081,7 +24081,7 @@
     </row>
     <row r="21" spans="1:13" ht="15.75" customHeight="1">
       <c r="A21" s="41" t="s">
-        <v>7524</v>
+        <v>7523</v>
       </c>
       <c r="B21" s="46" t="s">
         <v>7506</v>
@@ -24093,7 +24093,7 @@
         <v>43</v>
       </c>
       <c r="G21" s="41" t="s">
-        <v>7524</v>
+        <v>7523</v>
       </c>
       <c r="H21" s="18"/>
       <c r="I21" s="18" t="s">
@@ -24113,7 +24113,7 @@
     </row>
     <row r="22" spans="1:13" ht="15.75" customHeight="1">
       <c r="A22" s="41" t="s">
-        <v>7525</v>
+        <v>7524</v>
       </c>
       <c r="B22" s="46" t="s">
         <v>7506</v>
@@ -24125,7 +24125,7 @@
         <v>43</v>
       </c>
       <c r="G22" s="41" t="s">
-        <v>7525</v>
+        <v>7524</v>
       </c>
       <c r="H22" s="18"/>
       <c r="I22" s="18" t="s">
@@ -24145,7 +24145,7 @@
     </row>
     <row r="23" spans="1:13" ht="15.75" customHeight="1">
       <c r="A23" s="41" t="s">
-        <v>7526</v>
+        <v>7525</v>
       </c>
       <c r="B23" s="46" t="s">
         <v>7506</v>
@@ -24157,7 +24157,7 @@
         <v>43</v>
       </c>
       <c r="G23" s="41" t="s">
-        <v>7526</v>
+        <v>7525</v>
       </c>
       <c r="H23" s="18"/>
       <c r="I23" s="18" t="s">
@@ -24177,7 +24177,7 @@
     </row>
     <row r="24" spans="1:13" ht="15.75" customHeight="1">
       <c r="A24" s="41" t="s">
-        <v>7527</v>
+        <v>7526</v>
       </c>
       <c r="B24" s="46" t="s">
         <v>7506</v>
@@ -24189,7 +24189,7 @@
         <v>43</v>
       </c>
       <c r="G24" s="41" t="s">
-        <v>7527</v>
+        <v>7526</v>
       </c>
       <c r="H24" s="18"/>
       <c r="I24" s="18" t="s">
@@ -24209,7 +24209,7 @@
     </row>
     <row r="25" spans="1:13" ht="15.75" customHeight="1">
       <c r="A25" s="41" t="s">
-        <v>7528</v>
+        <v>7527</v>
       </c>
       <c r="B25" s="46" t="s">
         <v>7506</v>
@@ -24221,7 +24221,7 @@
         <v>43</v>
       </c>
       <c r="G25" s="41" t="s">
-        <v>7528</v>
+        <v>7527</v>
       </c>
       <c r="H25" s="18"/>
       <c r="I25" s="18" t="s">
@@ -24241,7 +24241,7 @@
     </row>
     <row r="26" spans="1:13" ht="15.75" customHeight="1">
       <c r="A26" s="41" t="s">
-        <v>7529</v>
+        <v>7528</v>
       </c>
       <c r="B26" s="46" t="s">
         <v>7506</v>
@@ -24253,7 +24253,7 @@
         <v>43</v>
       </c>
       <c r="G26" s="41" t="s">
-        <v>7529</v>
+        <v>7528</v>
       </c>
       <c r="H26" s="18"/>
       <c r="I26" s="18" t="s">
@@ -24273,7 +24273,7 @@
     </row>
     <row r="27" spans="1:13" ht="15.75" customHeight="1">
       <c r="A27" s="41" t="s">
-        <v>7530</v>
+        <v>7529</v>
       </c>
       <c r="B27" s="46" t="s">
         <v>7506</v>
@@ -24285,7 +24285,7 @@
         <v>43</v>
       </c>
       <c r="G27" s="41" t="s">
-        <v>7530</v>
+        <v>7529</v>
       </c>
       <c r="H27" s="18"/>
       <c r="I27" s="18" t="s">
@@ -24305,7 +24305,7 @@
     </row>
     <row r="28" spans="1:13" ht="15.75" customHeight="1">
       <c r="A28" s="41" t="s">
-        <v>7531</v>
+        <v>7530</v>
       </c>
       <c r="B28" s="46" t="s">
         <v>7506</v>
@@ -24317,7 +24317,7 @@
         <v>43</v>
       </c>
       <c r="G28" s="41" t="s">
-        <v>7531</v>
+        <v>7530</v>
       </c>
       <c r="H28" s="18"/>
       <c r="I28" s="18" t="s">
@@ -24337,7 +24337,7 @@
     </row>
     <row r="29" spans="1:13" ht="15.75" customHeight="1">
       <c r="A29" s="41" t="s">
-        <v>7532</v>
+        <v>7531</v>
       </c>
       <c r="B29" s="46" t="s">
         <v>7506</v>
@@ -24349,7 +24349,7 @@
         <v>43</v>
       </c>
       <c r="G29" s="41" t="s">
-        <v>7532</v>
+        <v>7531</v>
       </c>
       <c r="H29" s="18"/>
       <c r="I29" s="18" t="s">
@@ -24369,7 +24369,7 @@
     </row>
     <row r="30" spans="1:13" ht="15.75" customHeight="1">
       <c r="A30" s="41" t="s">
-        <v>7533</v>
+        <v>7532</v>
       </c>
       <c r="B30" s="46" t="s">
         <v>7506</v>
@@ -24381,7 +24381,7 @@
         <v>43</v>
       </c>
       <c r="G30" s="41" t="s">
-        <v>7533</v>
+        <v>7532</v>
       </c>
       <c r="H30" s="18"/>
       <c r="I30" s="18" t="s">
@@ -24401,7 +24401,7 @@
     </row>
     <row r="31" spans="1:13" ht="15.75" customHeight="1">
       <c r="A31" s="41" t="s">
-        <v>7534</v>
+        <v>7533</v>
       </c>
       <c r="B31" s="46" t="s">
         <v>7506</v>
@@ -24413,7 +24413,7 @@
         <v>43</v>
       </c>
       <c r="G31" s="41" t="s">
-        <v>7534</v>
+        <v>7533</v>
       </c>
       <c r="H31" s="18"/>
       <c r="I31" s="18" t="s">
@@ -24433,7 +24433,7 @@
     </row>
     <row r="32" spans="1:13" ht="15.75" customHeight="1">
       <c r="A32" s="41" t="s">
-        <v>7537</v>
+        <v>7536</v>
       </c>
       <c r="B32" s="46" t="s">
         <v>7506</v>
@@ -24445,7 +24445,7 @@
         <v>43</v>
       </c>
       <c r="G32" s="41" t="s">
-        <v>7537</v>
+        <v>7536</v>
       </c>
       <c r="H32" s="18"/>
       <c r="I32" s="18" t="s">
@@ -24465,7 +24465,7 @@
     </row>
     <row r="33" spans="1:13" ht="15.75" customHeight="1">
       <c r="A33" s="41" t="s">
-        <v>7535</v>
+        <v>7534</v>
       </c>
       <c r="B33" s="46" t="s">
         <v>7506</v>
@@ -24477,7 +24477,7 @@
         <v>43</v>
       </c>
       <c r="G33" s="41" t="s">
-        <v>7535</v>
+        <v>7534</v>
       </c>
       <c r="H33" s="18"/>
       <c r="I33" s="18" t="s">
@@ -24497,7 +24497,7 @@
     </row>
     <row r="34" spans="1:13" ht="15.75" customHeight="1">
       <c r="A34" s="41" t="s">
-        <v>7536</v>
+        <v>7535</v>
       </c>
       <c r="B34" s="46" t="s">
         <v>7506</v>
@@ -24509,7 +24509,7 @@
         <v>43</v>
       </c>
       <c r="G34" s="41" t="s">
-        <v>7536</v>
+        <v>7535</v>
       </c>
       <c r="H34" s="18"/>
       <c r="I34" s="18" t="s">
@@ -25628,7 +25628,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
@@ -26123,14 +26123,14 @@
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1">
       <c r="A14" s="45" t="s">
-        <v>7539</v>
+        <v>7538</v>
       </c>
       <c r="B14" s="21"/>
       <c r="D14" s="21" t="b">
         <v>1</v>
       </c>
       <c r="E14" s="41" t="s">
-        <v>7538</v>
+        <v>7537</v>
       </c>
       <c r="F14" s="18"/>
       <c r="G14" s="45" t="s">
@@ -73212,7 +73212,9 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -73225,7 +73227,7 @@
         <v>7514</v>
       </c>
       <c r="B1" s="39" t="s">
-        <v>7515</v>
+        <v>7539</v>
       </c>
       <c r="C1" s="33"/>
       <c r="D1" s="33"/>

</xml_diff>

<commit_message>
fix case on promoters
</commit_message>
<xml_diff>
--- a/Anderson Promoters/Anderson Promoters.xlsx
+++ b/Anderson Promoters/Anderson Promoters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakebeal/projects/BioTools/iGEM_distribution/Anderson Promoters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08F7BAF5-45FA-954E-A725-314E05F56F8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65947628-ABB9-1E47-8F03-2CBB715F22FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1780" yWindow="1300" windowWidth="34060" windowHeight="19800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23562,7 +23562,7 @@
   <dimension ref="A1:M983"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -23892,7 +23892,7 @@
         <v>7517</v>
       </c>
       <c r="B15" s="46" t="s">
-        <v>7505</v>
+        <v>41</v>
       </c>
       <c r="C15" s="18"/>
       <c r="D15" s="18"/>
@@ -23923,8 +23923,8 @@
       <c r="A16" s="45" t="s">
         <v>7506</v>
       </c>
-      <c r="B16" s="41" t="s">
-        <v>7505</v>
+      <c r="B16" s="46" t="s">
+        <v>41</v>
       </c>
       <c r="C16" s="21"/>
       <c r="D16" s="18"/>
@@ -23955,8 +23955,8 @@
       <c r="A17" s="41" t="s">
         <v>7518</v>
       </c>
-      <c r="B17" s="41" t="s">
-        <v>7505</v>
+      <c r="B17" s="46" t="s">
+        <v>41</v>
       </c>
       <c r="C17" s="18"/>
       <c r="D17" s="18"/>
@@ -23987,8 +23987,8 @@
       <c r="A18" s="41" t="s">
         <v>7519</v>
       </c>
-      <c r="B18" s="41" t="s">
-        <v>7505</v>
+      <c r="B18" s="46" t="s">
+        <v>41</v>
       </c>
       <c r="C18" s="18"/>
       <c r="D18" s="20"/>
@@ -24019,8 +24019,8 @@
       <c r="A19" s="41" t="s">
         <v>7520</v>
       </c>
-      <c r="B19" s="41" t="s">
-        <v>7505</v>
+      <c r="B19" s="46" t="s">
+        <v>41</v>
       </c>
       <c r="C19" s="18"/>
       <c r="D19" s="20"/>
@@ -24052,7 +24052,7 @@
         <v>7521</v>
       </c>
       <c r="B20" s="46" t="s">
-        <v>7505</v>
+        <v>41</v>
       </c>
       <c r="C20" s="18"/>
       <c r="D20" s="20"/>
@@ -24084,7 +24084,7 @@
         <v>7522</v>
       </c>
       <c r="B21" s="46" t="s">
-        <v>7505</v>
+        <v>41</v>
       </c>
       <c r="C21" s="18"/>
       <c r="D21" s="20"/>
@@ -24116,7 +24116,7 @@
         <v>7523</v>
       </c>
       <c r="B22" s="46" t="s">
-        <v>7505</v>
+        <v>41</v>
       </c>
       <c r="C22" s="18"/>
       <c r="D22" s="18"/>
@@ -24148,7 +24148,7 @@
         <v>7524</v>
       </c>
       <c r="B23" s="46" t="s">
-        <v>7505</v>
+        <v>41</v>
       </c>
       <c r="C23" s="18"/>
       <c r="D23" s="18"/>
@@ -24180,7 +24180,7 @@
         <v>7525</v>
       </c>
       <c r="B24" s="46" t="s">
-        <v>7505</v>
+        <v>41</v>
       </c>
       <c r="C24" s="18"/>
       <c r="D24" s="20"/>
@@ -24212,7 +24212,7 @@
         <v>7526</v>
       </c>
       <c r="B25" s="46" t="s">
-        <v>7505</v>
+        <v>41</v>
       </c>
       <c r="C25" s="18"/>
       <c r="D25" s="20"/>
@@ -24244,7 +24244,7 @@
         <v>7527</v>
       </c>
       <c r="B26" s="46" t="s">
-        <v>7505</v>
+        <v>41</v>
       </c>
       <c r="C26" s="18"/>
       <c r="D26" s="18"/>
@@ -24276,7 +24276,7 @@
         <v>7528</v>
       </c>
       <c r="B27" s="46" t="s">
-        <v>7505</v>
+        <v>41</v>
       </c>
       <c r="C27" s="18"/>
       <c r="D27" s="20"/>
@@ -24308,7 +24308,7 @@
         <v>7529</v>
       </c>
       <c r="B28" s="46" t="s">
-        <v>7505</v>
+        <v>41</v>
       </c>
       <c r="C28" s="18"/>
       <c r="D28" s="20"/>
@@ -24340,7 +24340,7 @@
         <v>7530</v>
       </c>
       <c r="B29" s="46" t="s">
-        <v>7505</v>
+        <v>41</v>
       </c>
       <c r="C29" s="18"/>
       <c r="D29" s="20"/>
@@ -24372,7 +24372,7 @@
         <v>7531</v>
       </c>
       <c r="B30" s="46" t="s">
-        <v>7505</v>
+        <v>41</v>
       </c>
       <c r="C30" s="21"/>
       <c r="D30" s="20"/>
@@ -24404,7 +24404,7 @@
         <v>7532</v>
       </c>
       <c r="B31" s="46" t="s">
-        <v>7505</v>
+        <v>41</v>
       </c>
       <c r="C31" s="18"/>
       <c r="D31" s="20"/>
@@ -24436,7 +24436,7 @@
         <v>7535</v>
       </c>
       <c r="B32" s="46" t="s">
-        <v>7505</v>
+        <v>41</v>
       </c>
       <c r="C32" s="18"/>
       <c r="D32" s="20"/>
@@ -24468,7 +24468,7 @@
         <v>7533</v>
       </c>
       <c r="B33" s="46" t="s">
-        <v>7505</v>
+        <v>41</v>
       </c>
       <c r="C33" s="18"/>
       <c r="D33" s="20"/>
@@ -24500,7 +24500,7 @@
         <v>7534</v>
       </c>
       <c r="B34" s="46" t="s">
-        <v>7505</v>
+        <v>41</v>
       </c>
       <c r="C34" s="18"/>
       <c r="D34" s="20"/>

</xml_diff>

<commit_message>
Move directory manipulation out of scriptutils/__init__.py to subpackage Update packages for sbol-utilities 1.05a
</commit_message>
<xml_diff>
--- a/Anderson Promoters/Anderson Promoters.xlsx
+++ b/Anderson Promoters/Anderson Promoters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakebeal/projects/BioTools/iGEM_distribution/Anderson Promoters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65947628-ABB9-1E47-8F03-2CBB715F22FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C1EE74A-3491-8E44-B746-E0B759639AB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1780" yWindow="1300" windowWidth="34060" windowHeight="19800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1780" yWindow="1300" windowWidth="34060" windowHeight="19800" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts and Devices" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7660" uniqueCount="7540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7661" uniqueCount="7542">
   <si>
     <t>Collection Name</t>
   </si>
@@ -22715,12 +22715,18 @@
   <si>
     <t>DNA Parts and Devices</t>
   </si>
+  <si>
+    <t>J23100, J23101, J23102, J23103, J23104, J23105, J23106, J23107, J23108, J23109, J23110, J23111, J23112, J23113, J23114, J23115, J23116, J23117, J23118, J23119</t>
+  </si>
+  <si>
+    <t>Literal Part</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="27">
+  <fonts count="28">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -22899,6 +22905,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -23047,7 +23059,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -23105,6 +23117,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -23561,7 +23574,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M983"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -25629,7 +25642,7 @@
   <dimension ref="A1:Z20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -26134,7 +26147,7 @@
       </c>
       <c r="F14" s="18"/>
       <c r="G14" s="45" t="s">
-        <v>7503</v>
+        <v>7540</v>
       </c>
       <c r="H14" s="18"/>
       <c r="I14" s="32"/>
@@ -71988,10 +72001,10 @@
   <sheetPr>
     <tabColor theme="8"/>
   </sheetPr>
-  <dimension ref="A1:F1000"/>
+  <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -72001,10 +72014,12 @@
     <col min="3" max="3" width="15.28515625" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" customWidth="1"/>
     <col min="5" max="5" width="21.28515625" customWidth="1"/>
-    <col min="6" max="26" width="8.7109375" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" style="40" customWidth="1"/>
+    <col min="8" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="37" t="s">
         <v>7462</v>
       </c>
@@ -72023,8 +72038,11 @@
       <c r="F1" s="37" t="s">
         <v>7467</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G1" s="33" t="s">
+        <v>7541</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="11" t="s">
         <v>7468</v>
       </c>
@@ -72043,8 +72061,11 @@
       <c r="F2" s="38" t="s">
         <v>7473</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G2" s="51" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="11" t="s">
         <v>7474</v>
       </c>
@@ -72063,8 +72084,11 @@
       <c r="F3" s="38" t="s">
         <v>7478</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G3" s="51" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" s="11" t="s">
         <v>7479</v>
       </c>
@@ -72083,8 +72107,11 @@
       <c r="F4" s="38" t="s">
         <v>7483</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G4" s="51" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" s="11" t="s">
         <v>7484</v>
       </c>
@@ -72103,8 +72130,11 @@
       <c r="F5" s="38" t="s">
         <v>7489</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G5" s="51" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" s="11" t="s">
         <v>8</v>
       </c>
@@ -72123,8 +72153,11 @@
       <c r="F6" s="38" t="s">
         <v>7494</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G6" s="51" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="A7" s="11" t="s">
         <v>7416</v>
       </c>
@@ -72143,1042 +72176,3024 @@
       <c r="F7" s="38" t="s">
         <v>7499</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G7" s="51" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="35"/>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G8" s="51"/>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G9" s="51"/>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G10" s="51"/>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G11" s="51"/>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G12" s="51"/>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G13" s="51"/>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="16" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="17" ht="15.75" customHeight="1"/>
-    <row r="18" ht="15.75" customHeight="1"/>
-    <row r="19" ht="15.75" customHeight="1"/>
-    <row r="20" ht="15.75" customHeight="1"/>
-    <row r="21" ht="15.75" customHeight="1"/>
-    <row r="22" ht="15.75" customHeight="1"/>
-    <row r="23" ht="15.75" customHeight="1"/>
-    <row r="24" ht="15.75" customHeight="1"/>
-    <row r="25" ht="15.75" customHeight="1"/>
-    <row r="26" ht="15.75" customHeight="1"/>
-    <row r="27" ht="15.75" customHeight="1"/>
-    <row r="28" ht="15.75" customHeight="1"/>
-    <row r="29" ht="15.75" customHeight="1"/>
-    <row r="30" ht="15.75" customHeight="1"/>
-    <row r="31" ht="15.75" customHeight="1"/>
-    <row r="32" ht="15.75" customHeight="1"/>
-    <row r="33" ht="15.75" customHeight="1"/>
-    <row r="34" ht="15.75" customHeight="1"/>
-    <row r="35" ht="15.75" customHeight="1"/>
-    <row r="36" ht="15.75" customHeight="1"/>
-    <row r="37" ht="15.75" customHeight="1"/>
-    <row r="38" ht="15.75" customHeight="1"/>
-    <row r="39" ht="15.75" customHeight="1"/>
-    <row r="40" ht="15.75" customHeight="1"/>
-    <row r="41" ht="15.75" customHeight="1"/>
-    <row r="42" ht="15.75" customHeight="1"/>
-    <row r="43" ht="15.75" customHeight="1"/>
-    <row r="44" ht="15.75" customHeight="1"/>
-    <row r="45" ht="15.75" customHeight="1"/>
-    <row r="46" ht="15.75" customHeight="1"/>
-    <row r="47" ht="15.75" customHeight="1"/>
-    <row r="48" ht="15.75" customHeight="1"/>
-    <row r="49" ht="15.75" customHeight="1"/>
-    <row r="50" ht="15.75" customHeight="1"/>
-    <row r="51" ht="15.75" customHeight="1"/>
-    <row r="52" ht="15.75" customHeight="1"/>
-    <row r="53" ht="15.75" customHeight="1"/>
-    <row r="54" ht="15.75" customHeight="1"/>
-    <row r="55" ht="15.75" customHeight="1"/>
-    <row r="56" ht="15.75" customHeight="1"/>
-    <row r="57" ht="15.75" customHeight="1"/>
-    <row r="58" ht="15.75" customHeight="1"/>
-    <row r="59" ht="15.75" customHeight="1"/>
-    <row r="60" ht="15.75" customHeight="1"/>
-    <row r="61" ht="15.75" customHeight="1"/>
-    <row r="62" ht="15.75" customHeight="1"/>
-    <row r="63" ht="15.75" customHeight="1"/>
-    <row r="64" ht="15.75" customHeight="1"/>
-    <row r="65" ht="15.75" customHeight="1"/>
-    <row r="66" ht="15.75" customHeight="1"/>
-    <row r="67" ht="15.75" customHeight="1"/>
-    <row r="68" ht="15.75" customHeight="1"/>
-    <row r="69" ht="15.75" customHeight="1"/>
-    <row r="70" ht="15.75" customHeight="1"/>
-    <row r="71" ht="15.75" customHeight="1"/>
-    <row r="72" ht="15.75" customHeight="1"/>
-    <row r="73" ht="15.75" customHeight="1"/>
-    <row r="74" ht="15.75" customHeight="1"/>
-    <row r="75" ht="15.75" customHeight="1"/>
-    <row r="76" ht="15.75" customHeight="1"/>
-    <row r="77" ht="15.75" customHeight="1"/>
-    <row r="78" ht="15.75" customHeight="1"/>
-    <row r="79" ht="15.75" customHeight="1"/>
-    <row r="80" ht="15.75" customHeight="1"/>
-    <row r="81" ht="15.75" customHeight="1"/>
-    <row r="82" ht="15.75" customHeight="1"/>
-    <row r="83" ht="15.75" customHeight="1"/>
-    <row r="84" ht="15.75" customHeight="1"/>
-    <row r="85" ht="15.75" customHeight="1"/>
-    <row r="86" ht="15.75" customHeight="1"/>
-    <row r="87" ht="15.75" customHeight="1"/>
-    <row r="88" ht="15.75" customHeight="1"/>
-    <row r="89" ht="15.75" customHeight="1"/>
-    <row r="90" ht="15.75" customHeight="1"/>
-    <row r="91" ht="15.75" customHeight="1"/>
-    <row r="92" ht="15.75" customHeight="1"/>
-    <row r="93" ht="15.75" customHeight="1"/>
-    <row r="94" ht="15.75" customHeight="1"/>
-    <row r="95" ht="15.75" customHeight="1"/>
-    <row r="96" ht="15.75" customHeight="1"/>
-    <row r="97" ht="15.75" customHeight="1"/>
-    <row r="98" ht="15.75" customHeight="1"/>
-    <row r="99" ht="15.75" customHeight="1"/>
-    <row r="100" ht="15.75" customHeight="1"/>
-    <row r="101" ht="15.75" customHeight="1"/>
-    <row r="102" ht="15.75" customHeight="1"/>
-    <row r="103" ht="15.75" customHeight="1"/>
-    <row r="104" ht="15.75" customHeight="1"/>
-    <row r="105" ht="15.75" customHeight="1"/>
-    <row r="106" ht="15.75" customHeight="1"/>
-    <row r="107" ht="15.75" customHeight="1"/>
-    <row r="108" ht="15.75" customHeight="1"/>
-    <row r="109" ht="15.75" customHeight="1"/>
-    <row r="110" ht="15.75" customHeight="1"/>
-    <row r="111" ht="15.75" customHeight="1"/>
-    <row r="112" ht="15.75" customHeight="1"/>
-    <row r="113" ht="15.75" customHeight="1"/>
-    <row r="114" ht="15.75" customHeight="1"/>
-    <row r="115" ht="15.75" customHeight="1"/>
-    <row r="116" ht="15.75" customHeight="1"/>
-    <row r="117" ht="15.75" customHeight="1"/>
-    <row r="118" ht="15.75" customHeight="1"/>
-    <row r="119" ht="15.75" customHeight="1"/>
-    <row r="120" ht="15.75" customHeight="1"/>
-    <row r="121" ht="15.75" customHeight="1"/>
-    <row r="122" ht="15.75" customHeight="1"/>
-    <row r="123" ht="15.75" customHeight="1"/>
-    <row r="124" ht="15.75" customHeight="1"/>
-    <row r="125" ht="15.75" customHeight="1"/>
-    <row r="126" ht="15.75" customHeight="1"/>
-    <row r="127" ht="15.75" customHeight="1"/>
-    <row r="128" ht="15.75" customHeight="1"/>
-    <row r="129" ht="15.75" customHeight="1"/>
-    <row r="130" ht="15.75" customHeight="1"/>
-    <row r="131" ht="15.75" customHeight="1"/>
-    <row r="132" ht="15.75" customHeight="1"/>
-    <row r="133" ht="15.75" customHeight="1"/>
-    <row r="134" ht="15.75" customHeight="1"/>
-    <row r="135" ht="15.75" customHeight="1"/>
-    <row r="136" ht="15.75" customHeight="1"/>
-    <row r="137" ht="15.75" customHeight="1"/>
-    <row r="138" ht="15.75" customHeight="1"/>
-    <row r="139" ht="15.75" customHeight="1"/>
-    <row r="140" ht="15.75" customHeight="1"/>
-    <row r="141" ht="15.75" customHeight="1"/>
-    <row r="142" ht="15.75" customHeight="1"/>
-    <row r="143" ht="15.75" customHeight="1"/>
-    <row r="144" ht="15.75" customHeight="1"/>
-    <row r="145" ht="15.75" customHeight="1"/>
-    <row r="146" ht="15.75" customHeight="1"/>
-    <row r="147" ht="15.75" customHeight="1"/>
-    <row r="148" ht="15.75" customHeight="1"/>
-    <row r="149" ht="15.75" customHeight="1"/>
-    <row r="150" ht="15.75" customHeight="1"/>
-    <row r="151" ht="15.75" customHeight="1"/>
-    <row r="152" ht="15.75" customHeight="1"/>
-    <row r="153" ht="15.75" customHeight="1"/>
-    <row r="154" ht="15.75" customHeight="1"/>
-    <row r="155" ht="15.75" customHeight="1"/>
-    <row r="156" ht="15.75" customHeight="1"/>
-    <row r="157" ht="15.75" customHeight="1"/>
-    <row r="158" ht="15.75" customHeight="1"/>
-    <row r="159" ht="15.75" customHeight="1"/>
-    <row r="160" ht="15.75" customHeight="1"/>
-    <row r="161" ht="15.75" customHeight="1"/>
-    <row r="162" ht="15.75" customHeight="1"/>
-    <row r="163" ht="15.75" customHeight="1"/>
-    <row r="164" ht="15.75" customHeight="1"/>
-    <row r="165" ht="15.75" customHeight="1"/>
-    <row r="166" ht="15.75" customHeight="1"/>
-    <row r="167" ht="15.75" customHeight="1"/>
-    <row r="168" ht="15.75" customHeight="1"/>
-    <row r="169" ht="15.75" customHeight="1"/>
-    <row r="170" ht="15.75" customHeight="1"/>
-    <row r="171" ht="15.75" customHeight="1"/>
-    <row r="172" ht="15.75" customHeight="1"/>
-    <row r="173" ht="15.75" customHeight="1"/>
-    <row r="174" ht="15.75" customHeight="1"/>
-    <row r="175" ht="15.75" customHeight="1"/>
-    <row r="176" ht="15.75" customHeight="1"/>
-    <row r="177" ht="15.75" customHeight="1"/>
-    <row r="178" ht="15.75" customHeight="1"/>
-    <row r="179" ht="15.75" customHeight="1"/>
-    <row r="180" ht="15.75" customHeight="1"/>
-    <row r="181" ht="15.75" customHeight="1"/>
-    <row r="182" ht="15.75" customHeight="1"/>
-    <row r="183" ht="15.75" customHeight="1"/>
-    <row r="184" ht="15.75" customHeight="1"/>
-    <row r="185" ht="15.75" customHeight="1"/>
-    <row r="186" ht="15.75" customHeight="1"/>
-    <row r="187" ht="15.75" customHeight="1"/>
-    <row r="188" ht="15.75" customHeight="1"/>
-    <row r="189" ht="15.75" customHeight="1"/>
-    <row r="190" ht="15.75" customHeight="1"/>
-    <row r="191" ht="15.75" customHeight="1"/>
-    <row r="192" ht="15.75" customHeight="1"/>
-    <row r="193" ht="15.75" customHeight="1"/>
-    <row r="194" ht="15.75" customHeight="1"/>
-    <row r="195" ht="15.75" customHeight="1"/>
-    <row r="196" ht="15.75" customHeight="1"/>
-    <row r="197" ht="15.75" customHeight="1"/>
-    <row r="198" ht="15.75" customHeight="1"/>
-    <row r="199" ht="15.75" customHeight="1"/>
-    <row r="200" ht="15.75" customHeight="1"/>
-    <row r="201" ht="15.75" customHeight="1"/>
-    <row r="202" ht="15.75" customHeight="1"/>
-    <row r="203" ht="15.75" customHeight="1"/>
-    <row r="204" ht="15.75" customHeight="1"/>
-    <row r="205" ht="15.75" customHeight="1"/>
-    <row r="206" ht="15.75" customHeight="1"/>
-    <row r="207" ht="15.75" customHeight="1"/>
-    <row r="208" ht="15.75" customHeight="1"/>
-    <row r="209" ht="15.75" customHeight="1"/>
-    <row r="210" ht="15.75" customHeight="1"/>
-    <row r="211" ht="15.75" customHeight="1"/>
-    <row r="212" ht="15.75" customHeight="1"/>
-    <row r="213" ht="15.75" customHeight="1"/>
-    <row r="214" ht="15.75" customHeight="1"/>
-    <row r="215" ht="15.75" customHeight="1"/>
-    <row r="216" ht="15.75" customHeight="1"/>
-    <row r="217" ht="15.75" customHeight="1"/>
-    <row r="218" ht="15.75" customHeight="1"/>
-    <row r="219" ht="15.75" customHeight="1"/>
-    <row r="220" ht="15.75" customHeight="1"/>
-    <row r="221" ht="15.75" customHeight="1"/>
-    <row r="222" ht="15.75" customHeight="1"/>
-    <row r="223" ht="15.75" customHeight="1"/>
-    <row r="224" ht="15.75" customHeight="1"/>
-    <row r="225" ht="15.75" customHeight="1"/>
-    <row r="226" ht="15.75" customHeight="1"/>
-    <row r="227" ht="15.75" customHeight="1"/>
-    <row r="228" ht="15.75" customHeight="1"/>
-    <row r="229" ht="15.75" customHeight="1"/>
-    <row r="230" ht="15.75" customHeight="1"/>
-    <row r="231" ht="15.75" customHeight="1"/>
-    <row r="232" ht="15.75" customHeight="1"/>
-    <row r="233" ht="15.75" customHeight="1"/>
-    <row r="234" ht="15.75" customHeight="1"/>
-    <row r="235" ht="15.75" customHeight="1"/>
-    <row r="236" ht="15.75" customHeight="1"/>
-    <row r="237" ht="15.75" customHeight="1"/>
-    <row r="238" ht="15.75" customHeight="1"/>
-    <row r="239" ht="15.75" customHeight="1"/>
-    <row r="240" ht="15.75" customHeight="1"/>
-    <row r="241" ht="15.75" customHeight="1"/>
-    <row r="242" ht="15.75" customHeight="1"/>
-    <row r="243" ht="15.75" customHeight="1"/>
-    <row r="244" ht="15.75" customHeight="1"/>
-    <row r="245" ht="15.75" customHeight="1"/>
-    <row r="246" ht="15.75" customHeight="1"/>
-    <row r="247" ht="15.75" customHeight="1"/>
-    <row r="248" ht="15.75" customHeight="1"/>
-    <row r="249" ht="15.75" customHeight="1"/>
-    <row r="250" ht="15.75" customHeight="1"/>
-    <row r="251" ht="15.75" customHeight="1"/>
-    <row r="252" ht="15.75" customHeight="1"/>
-    <row r="253" ht="15.75" customHeight="1"/>
-    <row r="254" ht="15.75" customHeight="1"/>
-    <row r="255" ht="15.75" customHeight="1"/>
-    <row r="256" ht="15.75" customHeight="1"/>
-    <row r="257" ht="15.75" customHeight="1"/>
-    <row r="258" ht="15.75" customHeight="1"/>
-    <row r="259" ht="15.75" customHeight="1"/>
-    <row r="260" ht="15.75" customHeight="1"/>
-    <row r="261" ht="15.75" customHeight="1"/>
-    <row r="262" ht="15.75" customHeight="1"/>
-    <row r="263" ht="15.75" customHeight="1"/>
-    <row r="264" ht="15.75" customHeight="1"/>
-    <row r="265" ht="15.75" customHeight="1"/>
-    <row r="266" ht="15.75" customHeight="1"/>
-    <row r="267" ht="15.75" customHeight="1"/>
-    <row r="268" ht="15.75" customHeight="1"/>
-    <row r="269" ht="15.75" customHeight="1"/>
-    <row r="270" ht="15.75" customHeight="1"/>
-    <row r="271" ht="15.75" customHeight="1"/>
-    <row r="272" ht="15.75" customHeight="1"/>
-    <row r="273" ht="15.75" customHeight="1"/>
-    <row r="274" ht="15.75" customHeight="1"/>
-    <row r="275" ht="15.75" customHeight="1"/>
-    <row r="276" ht="15.75" customHeight="1"/>
-    <row r="277" ht="15.75" customHeight="1"/>
-    <row r="278" ht="15.75" customHeight="1"/>
-    <row r="279" ht="15.75" customHeight="1"/>
-    <row r="280" ht="15.75" customHeight="1"/>
-    <row r="281" ht="15.75" customHeight="1"/>
-    <row r="282" ht="15.75" customHeight="1"/>
-    <row r="283" ht="15.75" customHeight="1"/>
-    <row r="284" ht="15.75" customHeight="1"/>
-    <row r="285" ht="15.75" customHeight="1"/>
-    <row r="286" ht="15.75" customHeight="1"/>
-    <row r="287" ht="15.75" customHeight="1"/>
-    <row r="288" ht="15.75" customHeight="1"/>
-    <row r="289" ht="15.75" customHeight="1"/>
-    <row r="290" ht="15.75" customHeight="1"/>
-    <row r="291" ht="15.75" customHeight="1"/>
-    <row r="292" ht="15.75" customHeight="1"/>
-    <row r="293" ht="15.75" customHeight="1"/>
-    <row r="294" ht="15.75" customHeight="1"/>
-    <row r="295" ht="15.75" customHeight="1"/>
-    <row r="296" ht="15.75" customHeight="1"/>
-    <row r="297" ht="15.75" customHeight="1"/>
-    <row r="298" ht="15.75" customHeight="1"/>
-    <row r="299" ht="15.75" customHeight="1"/>
-    <row r="300" ht="15.75" customHeight="1"/>
-    <row r="301" ht="15.75" customHeight="1"/>
-    <row r="302" ht="15.75" customHeight="1"/>
-    <row r="303" ht="15.75" customHeight="1"/>
-    <row r="304" ht="15.75" customHeight="1"/>
-    <row r="305" ht="15.75" customHeight="1"/>
-    <row r="306" ht="15.75" customHeight="1"/>
-    <row r="307" ht="15.75" customHeight="1"/>
-    <row r="308" ht="15.75" customHeight="1"/>
-    <row r="309" ht="15.75" customHeight="1"/>
-    <row r="310" ht="15.75" customHeight="1"/>
-    <row r="311" ht="15.75" customHeight="1"/>
-    <row r="312" ht="15.75" customHeight="1"/>
-    <row r="313" ht="15.75" customHeight="1"/>
-    <row r="314" ht="15.75" customHeight="1"/>
-    <row r="315" ht="15.75" customHeight="1"/>
-    <row r="316" ht="15.75" customHeight="1"/>
-    <row r="317" ht="15.75" customHeight="1"/>
-    <row r="318" ht="15.75" customHeight="1"/>
-    <row r="319" ht="15.75" customHeight="1"/>
-    <row r="320" ht="15.75" customHeight="1"/>
-    <row r="321" ht="15.75" customHeight="1"/>
-    <row r="322" ht="15.75" customHeight="1"/>
-    <row r="323" ht="15.75" customHeight="1"/>
-    <row r="324" ht="15.75" customHeight="1"/>
-    <row r="325" ht="15.75" customHeight="1"/>
-    <row r="326" ht="15.75" customHeight="1"/>
-    <row r="327" ht="15.75" customHeight="1"/>
-    <row r="328" ht="15.75" customHeight="1"/>
-    <row r="329" ht="15.75" customHeight="1"/>
-    <row r="330" ht="15.75" customHeight="1"/>
-    <row r="331" ht="15.75" customHeight="1"/>
-    <row r="332" ht="15.75" customHeight="1"/>
-    <row r="333" ht="15.75" customHeight="1"/>
-    <row r="334" ht="15.75" customHeight="1"/>
-    <row r="335" ht="15.75" customHeight="1"/>
-    <row r="336" ht="15.75" customHeight="1"/>
-    <row r="337" ht="15.75" customHeight="1"/>
-    <row r="338" ht="15.75" customHeight="1"/>
-    <row r="339" ht="15.75" customHeight="1"/>
-    <row r="340" ht="15.75" customHeight="1"/>
-    <row r="341" ht="15.75" customHeight="1"/>
-    <row r="342" ht="15.75" customHeight="1"/>
-    <row r="343" ht="15.75" customHeight="1"/>
-    <row r="344" ht="15.75" customHeight="1"/>
-    <row r="345" ht="15.75" customHeight="1"/>
-    <row r="346" ht="15.75" customHeight="1"/>
-    <row r="347" ht="15.75" customHeight="1"/>
-    <row r="348" ht="15.75" customHeight="1"/>
-    <row r="349" ht="15.75" customHeight="1"/>
-    <row r="350" ht="15.75" customHeight="1"/>
-    <row r="351" ht="15.75" customHeight="1"/>
-    <row r="352" ht="15.75" customHeight="1"/>
-    <row r="353" ht="15.75" customHeight="1"/>
-    <row r="354" ht="15.75" customHeight="1"/>
-    <row r="355" ht="15.75" customHeight="1"/>
-    <row r="356" ht="15.75" customHeight="1"/>
-    <row r="357" ht="15.75" customHeight="1"/>
-    <row r="358" ht="15.75" customHeight="1"/>
-    <row r="359" ht="15.75" customHeight="1"/>
-    <row r="360" ht="15.75" customHeight="1"/>
-    <row r="361" ht="15.75" customHeight="1"/>
-    <row r="362" ht="15.75" customHeight="1"/>
-    <row r="363" ht="15.75" customHeight="1"/>
-    <row r="364" ht="15.75" customHeight="1"/>
-    <row r="365" ht="15.75" customHeight="1"/>
-    <row r="366" ht="15.75" customHeight="1"/>
-    <row r="367" ht="15.75" customHeight="1"/>
-    <row r="368" ht="15.75" customHeight="1"/>
-    <row r="369" ht="15.75" customHeight="1"/>
-    <row r="370" ht="15.75" customHeight="1"/>
-    <row r="371" ht="15.75" customHeight="1"/>
-    <row r="372" ht="15.75" customHeight="1"/>
-    <row r="373" ht="15.75" customHeight="1"/>
-    <row r="374" ht="15.75" customHeight="1"/>
-    <row r="375" ht="15.75" customHeight="1"/>
-    <row r="376" ht="15.75" customHeight="1"/>
-    <row r="377" ht="15.75" customHeight="1"/>
-    <row r="378" ht="15.75" customHeight="1"/>
-    <row r="379" ht="15.75" customHeight="1"/>
-    <row r="380" ht="15.75" customHeight="1"/>
-    <row r="381" ht="15.75" customHeight="1"/>
-    <row r="382" ht="15.75" customHeight="1"/>
-    <row r="383" ht="15.75" customHeight="1"/>
-    <row r="384" ht="15.75" customHeight="1"/>
-    <row r="385" ht="15.75" customHeight="1"/>
-    <row r="386" ht="15.75" customHeight="1"/>
-    <row r="387" ht="15.75" customHeight="1"/>
-    <row r="388" ht="15.75" customHeight="1"/>
-    <row r="389" ht="15.75" customHeight="1"/>
-    <row r="390" ht="15.75" customHeight="1"/>
-    <row r="391" ht="15.75" customHeight="1"/>
-    <row r="392" ht="15.75" customHeight="1"/>
-    <row r="393" ht="15.75" customHeight="1"/>
-    <row r="394" ht="15.75" customHeight="1"/>
-    <row r="395" ht="15.75" customHeight="1"/>
-    <row r="396" ht="15.75" customHeight="1"/>
-    <row r="397" ht="15.75" customHeight="1"/>
-    <row r="398" ht="15.75" customHeight="1"/>
-    <row r="399" ht="15.75" customHeight="1"/>
-    <row r="400" ht="15.75" customHeight="1"/>
-    <row r="401" ht="15.75" customHeight="1"/>
-    <row r="402" ht="15.75" customHeight="1"/>
-    <row r="403" ht="15.75" customHeight="1"/>
-    <row r="404" ht="15.75" customHeight="1"/>
-    <row r="405" ht="15.75" customHeight="1"/>
-    <row r="406" ht="15.75" customHeight="1"/>
-    <row r="407" ht="15.75" customHeight="1"/>
-    <row r="408" ht="15.75" customHeight="1"/>
-    <row r="409" ht="15.75" customHeight="1"/>
-    <row r="410" ht="15.75" customHeight="1"/>
-    <row r="411" ht="15.75" customHeight="1"/>
-    <row r="412" ht="15.75" customHeight="1"/>
-    <row r="413" ht="15.75" customHeight="1"/>
-    <row r="414" ht="15.75" customHeight="1"/>
-    <row r="415" ht="15.75" customHeight="1"/>
-    <row r="416" ht="15.75" customHeight="1"/>
-    <row r="417" ht="15.75" customHeight="1"/>
-    <row r="418" ht="15.75" customHeight="1"/>
-    <row r="419" ht="15.75" customHeight="1"/>
-    <row r="420" ht="15.75" customHeight="1"/>
-    <row r="421" ht="15.75" customHeight="1"/>
-    <row r="422" ht="15.75" customHeight="1"/>
-    <row r="423" ht="15.75" customHeight="1"/>
-    <row r="424" ht="15.75" customHeight="1"/>
-    <row r="425" ht="15.75" customHeight="1"/>
-    <row r="426" ht="15.75" customHeight="1"/>
-    <row r="427" ht="15.75" customHeight="1"/>
-    <row r="428" ht="15.75" customHeight="1"/>
-    <row r="429" ht="15.75" customHeight="1"/>
-    <row r="430" ht="15.75" customHeight="1"/>
-    <row r="431" ht="15.75" customHeight="1"/>
-    <row r="432" ht="15.75" customHeight="1"/>
-    <row r="433" ht="15.75" customHeight="1"/>
-    <row r="434" ht="15.75" customHeight="1"/>
-    <row r="435" ht="15.75" customHeight="1"/>
-    <row r="436" ht="15.75" customHeight="1"/>
-    <row r="437" ht="15.75" customHeight="1"/>
-    <row r="438" ht="15.75" customHeight="1"/>
-    <row r="439" ht="15.75" customHeight="1"/>
-    <row r="440" ht="15.75" customHeight="1"/>
-    <row r="441" ht="15.75" customHeight="1"/>
-    <row r="442" ht="15.75" customHeight="1"/>
-    <row r="443" ht="15.75" customHeight="1"/>
-    <row r="444" ht="15.75" customHeight="1"/>
-    <row r="445" ht="15.75" customHeight="1"/>
-    <row r="446" ht="15.75" customHeight="1"/>
-    <row r="447" ht="15.75" customHeight="1"/>
-    <row r="448" ht="15.75" customHeight="1"/>
-    <row r="449" ht="15.75" customHeight="1"/>
-    <row r="450" ht="15.75" customHeight="1"/>
-    <row r="451" ht="15.75" customHeight="1"/>
-    <row r="452" ht="15.75" customHeight="1"/>
-    <row r="453" ht="15.75" customHeight="1"/>
-    <row r="454" ht="15.75" customHeight="1"/>
-    <row r="455" ht="15.75" customHeight="1"/>
-    <row r="456" ht="15.75" customHeight="1"/>
-    <row r="457" ht="15.75" customHeight="1"/>
-    <row r="458" ht="15.75" customHeight="1"/>
-    <row r="459" ht="15.75" customHeight="1"/>
-    <row r="460" ht="15.75" customHeight="1"/>
-    <row r="461" ht="15.75" customHeight="1"/>
-    <row r="462" ht="15.75" customHeight="1"/>
-    <row r="463" ht="15.75" customHeight="1"/>
-    <row r="464" ht="15.75" customHeight="1"/>
-    <row r="465" ht="15.75" customHeight="1"/>
-    <row r="466" ht="15.75" customHeight="1"/>
-    <row r="467" ht="15.75" customHeight="1"/>
-    <row r="468" ht="15.75" customHeight="1"/>
-    <row r="469" ht="15.75" customHeight="1"/>
-    <row r="470" ht="15.75" customHeight="1"/>
-    <row r="471" ht="15.75" customHeight="1"/>
-    <row r="472" ht="15.75" customHeight="1"/>
-    <row r="473" ht="15.75" customHeight="1"/>
-    <row r="474" ht="15.75" customHeight="1"/>
-    <row r="475" ht="15.75" customHeight="1"/>
-    <row r="476" ht="15.75" customHeight="1"/>
-    <row r="477" ht="15.75" customHeight="1"/>
-    <row r="478" ht="15.75" customHeight="1"/>
-    <row r="479" ht="15.75" customHeight="1"/>
-    <row r="480" ht="15.75" customHeight="1"/>
-    <row r="481" ht="15.75" customHeight="1"/>
-    <row r="482" ht="15.75" customHeight="1"/>
-    <row r="483" ht="15.75" customHeight="1"/>
-    <row r="484" ht="15.75" customHeight="1"/>
-    <row r="485" ht="15.75" customHeight="1"/>
-    <row r="486" ht="15.75" customHeight="1"/>
-    <row r="487" ht="15.75" customHeight="1"/>
-    <row r="488" ht="15.75" customHeight="1"/>
-    <row r="489" ht="15.75" customHeight="1"/>
-    <row r="490" ht="15.75" customHeight="1"/>
-    <row r="491" ht="15.75" customHeight="1"/>
-    <row r="492" ht="15.75" customHeight="1"/>
-    <row r="493" ht="15.75" customHeight="1"/>
-    <row r="494" ht="15.75" customHeight="1"/>
-    <row r="495" ht="15.75" customHeight="1"/>
-    <row r="496" ht="15.75" customHeight="1"/>
-    <row r="497" ht="15.75" customHeight="1"/>
-    <row r="498" ht="15.75" customHeight="1"/>
-    <row r="499" ht="15.75" customHeight="1"/>
-    <row r="500" ht="15.75" customHeight="1"/>
-    <row r="501" ht="15.75" customHeight="1"/>
-    <row r="502" ht="15.75" customHeight="1"/>
-    <row r="503" ht="15.75" customHeight="1"/>
-    <row r="504" ht="15.75" customHeight="1"/>
-    <row r="505" ht="15.75" customHeight="1"/>
-    <row r="506" ht="15.75" customHeight="1"/>
-    <row r="507" ht="15.75" customHeight="1"/>
-    <row r="508" ht="15.75" customHeight="1"/>
-    <row r="509" ht="15.75" customHeight="1"/>
-    <row r="510" ht="15.75" customHeight="1"/>
-    <row r="511" ht="15.75" customHeight="1"/>
-    <row r="512" ht="15.75" customHeight="1"/>
-    <row r="513" ht="15.75" customHeight="1"/>
-    <row r="514" ht="15.75" customHeight="1"/>
-    <row r="515" ht="15.75" customHeight="1"/>
-    <row r="516" ht="15.75" customHeight="1"/>
-    <row r="517" ht="15.75" customHeight="1"/>
-    <row r="518" ht="15.75" customHeight="1"/>
-    <row r="519" ht="15.75" customHeight="1"/>
-    <row r="520" ht="15.75" customHeight="1"/>
-    <row r="521" ht="15.75" customHeight="1"/>
-    <row r="522" ht="15.75" customHeight="1"/>
-    <row r="523" ht="15.75" customHeight="1"/>
-    <row r="524" ht="15.75" customHeight="1"/>
-    <row r="525" ht="15.75" customHeight="1"/>
-    <row r="526" ht="15.75" customHeight="1"/>
-    <row r="527" ht="15.75" customHeight="1"/>
-    <row r="528" ht="15.75" customHeight="1"/>
-    <row r="529" ht="15.75" customHeight="1"/>
-    <row r="530" ht="15.75" customHeight="1"/>
-    <row r="531" ht="15.75" customHeight="1"/>
-    <row r="532" ht="15.75" customHeight="1"/>
-    <row r="533" ht="15.75" customHeight="1"/>
-    <row r="534" ht="15.75" customHeight="1"/>
-    <row r="535" ht="15.75" customHeight="1"/>
-    <row r="536" ht="15.75" customHeight="1"/>
-    <row r="537" ht="15.75" customHeight="1"/>
-    <row r="538" ht="15.75" customHeight="1"/>
-    <row r="539" ht="15.75" customHeight="1"/>
-    <row r="540" ht="15.75" customHeight="1"/>
-    <row r="541" ht="15.75" customHeight="1"/>
-    <row r="542" ht="15.75" customHeight="1"/>
-    <row r="543" ht="15.75" customHeight="1"/>
-    <row r="544" ht="15.75" customHeight="1"/>
-    <row r="545" ht="15.75" customHeight="1"/>
-    <row r="546" ht="15.75" customHeight="1"/>
-    <row r="547" ht="15.75" customHeight="1"/>
-    <row r="548" ht="15.75" customHeight="1"/>
-    <row r="549" ht="15.75" customHeight="1"/>
-    <row r="550" ht="15.75" customHeight="1"/>
-    <row r="551" ht="15.75" customHeight="1"/>
-    <row r="552" ht="15.75" customHeight="1"/>
-    <row r="553" ht="15.75" customHeight="1"/>
-    <row r="554" ht="15.75" customHeight="1"/>
-    <row r="555" ht="15.75" customHeight="1"/>
-    <row r="556" ht="15.75" customHeight="1"/>
-    <row r="557" ht="15.75" customHeight="1"/>
-    <row r="558" ht="15.75" customHeight="1"/>
-    <row r="559" ht="15.75" customHeight="1"/>
-    <row r="560" ht="15.75" customHeight="1"/>
-    <row r="561" ht="15.75" customHeight="1"/>
-    <row r="562" ht="15.75" customHeight="1"/>
-    <row r="563" ht="15.75" customHeight="1"/>
-    <row r="564" ht="15.75" customHeight="1"/>
-    <row r="565" ht="15.75" customHeight="1"/>
-    <row r="566" ht="15.75" customHeight="1"/>
-    <row r="567" ht="15.75" customHeight="1"/>
-    <row r="568" ht="15.75" customHeight="1"/>
-    <row r="569" ht="15.75" customHeight="1"/>
-    <row r="570" ht="15.75" customHeight="1"/>
-    <row r="571" ht="15.75" customHeight="1"/>
-    <row r="572" ht="15.75" customHeight="1"/>
-    <row r="573" ht="15.75" customHeight="1"/>
-    <row r="574" ht="15.75" customHeight="1"/>
-    <row r="575" ht="15.75" customHeight="1"/>
-    <row r="576" ht="15.75" customHeight="1"/>
-    <row r="577" ht="15.75" customHeight="1"/>
-    <row r="578" ht="15.75" customHeight="1"/>
-    <row r="579" ht="15.75" customHeight="1"/>
-    <row r="580" ht="15.75" customHeight="1"/>
-    <row r="581" ht="15.75" customHeight="1"/>
-    <row r="582" ht="15.75" customHeight="1"/>
-    <row r="583" ht="15.75" customHeight="1"/>
-    <row r="584" ht="15.75" customHeight="1"/>
-    <row r="585" ht="15.75" customHeight="1"/>
-    <row r="586" ht="15.75" customHeight="1"/>
-    <row r="587" ht="15.75" customHeight="1"/>
-    <row r="588" ht="15.75" customHeight="1"/>
-    <row r="589" ht="15.75" customHeight="1"/>
-    <row r="590" ht="15.75" customHeight="1"/>
-    <row r="591" ht="15.75" customHeight="1"/>
-    <row r="592" ht="15.75" customHeight="1"/>
-    <row r="593" ht="15.75" customHeight="1"/>
-    <row r="594" ht="15.75" customHeight="1"/>
-    <row r="595" ht="15.75" customHeight="1"/>
-    <row r="596" ht="15.75" customHeight="1"/>
-    <row r="597" ht="15.75" customHeight="1"/>
-    <row r="598" ht="15.75" customHeight="1"/>
-    <row r="599" ht="15.75" customHeight="1"/>
-    <row r="600" ht="15.75" customHeight="1"/>
-    <row r="601" ht="15.75" customHeight="1"/>
-    <row r="602" ht="15.75" customHeight="1"/>
-    <row r="603" ht="15.75" customHeight="1"/>
-    <row r="604" ht="15.75" customHeight="1"/>
-    <row r="605" ht="15.75" customHeight="1"/>
-    <row r="606" ht="15.75" customHeight="1"/>
-    <row r="607" ht="15.75" customHeight="1"/>
-    <row r="608" ht="15.75" customHeight="1"/>
-    <row r="609" ht="15.75" customHeight="1"/>
-    <row r="610" ht="15.75" customHeight="1"/>
-    <row r="611" ht="15.75" customHeight="1"/>
-    <row r="612" ht="15.75" customHeight="1"/>
-    <row r="613" ht="15.75" customHeight="1"/>
-    <row r="614" ht="15.75" customHeight="1"/>
-    <row r="615" ht="15.75" customHeight="1"/>
-    <row r="616" ht="15.75" customHeight="1"/>
-    <row r="617" ht="15.75" customHeight="1"/>
-    <row r="618" ht="15.75" customHeight="1"/>
-    <row r="619" ht="15.75" customHeight="1"/>
-    <row r="620" ht="15.75" customHeight="1"/>
-    <row r="621" ht="15.75" customHeight="1"/>
-    <row r="622" ht="15.75" customHeight="1"/>
-    <row r="623" ht="15.75" customHeight="1"/>
-    <row r="624" ht="15.75" customHeight="1"/>
-    <row r="625" ht="15.75" customHeight="1"/>
-    <row r="626" ht="15.75" customHeight="1"/>
-    <row r="627" ht="15.75" customHeight="1"/>
-    <row r="628" ht="15.75" customHeight="1"/>
-    <row r="629" ht="15.75" customHeight="1"/>
-    <row r="630" ht="15.75" customHeight="1"/>
-    <row r="631" ht="15.75" customHeight="1"/>
-    <row r="632" ht="15.75" customHeight="1"/>
-    <row r="633" ht="15.75" customHeight="1"/>
-    <row r="634" ht="15.75" customHeight="1"/>
-    <row r="635" ht="15.75" customHeight="1"/>
-    <row r="636" ht="15.75" customHeight="1"/>
-    <row r="637" ht="15.75" customHeight="1"/>
-    <row r="638" ht="15.75" customHeight="1"/>
-    <row r="639" ht="15.75" customHeight="1"/>
-    <row r="640" ht="15.75" customHeight="1"/>
-    <row r="641" ht="15.75" customHeight="1"/>
-    <row r="642" ht="15.75" customHeight="1"/>
-    <row r="643" ht="15.75" customHeight="1"/>
-    <row r="644" ht="15.75" customHeight="1"/>
-    <row r="645" ht="15.75" customHeight="1"/>
-    <row r="646" ht="15.75" customHeight="1"/>
-    <row r="647" ht="15.75" customHeight="1"/>
-    <row r="648" ht="15.75" customHeight="1"/>
-    <row r="649" ht="15.75" customHeight="1"/>
-    <row r="650" ht="15.75" customHeight="1"/>
-    <row r="651" ht="15.75" customHeight="1"/>
-    <row r="652" ht="15.75" customHeight="1"/>
-    <row r="653" ht="15.75" customHeight="1"/>
-    <row r="654" ht="15.75" customHeight="1"/>
-    <row r="655" ht="15.75" customHeight="1"/>
-    <row r="656" ht="15.75" customHeight="1"/>
-    <row r="657" ht="15.75" customHeight="1"/>
-    <row r="658" ht="15.75" customHeight="1"/>
-    <row r="659" ht="15.75" customHeight="1"/>
-    <row r="660" ht="15.75" customHeight="1"/>
-    <row r="661" ht="15.75" customHeight="1"/>
-    <row r="662" ht="15.75" customHeight="1"/>
-    <row r="663" ht="15.75" customHeight="1"/>
-    <row r="664" ht="15.75" customHeight="1"/>
-    <row r="665" ht="15.75" customHeight="1"/>
-    <row r="666" ht="15.75" customHeight="1"/>
-    <row r="667" ht="15.75" customHeight="1"/>
-    <row r="668" ht="15.75" customHeight="1"/>
-    <row r="669" ht="15.75" customHeight="1"/>
-    <row r="670" ht="15.75" customHeight="1"/>
-    <row r="671" ht="15.75" customHeight="1"/>
-    <row r="672" ht="15.75" customHeight="1"/>
-    <row r="673" ht="15.75" customHeight="1"/>
-    <row r="674" ht="15.75" customHeight="1"/>
-    <row r="675" ht="15.75" customHeight="1"/>
-    <row r="676" ht="15.75" customHeight="1"/>
-    <row r="677" ht="15.75" customHeight="1"/>
-    <row r="678" ht="15.75" customHeight="1"/>
-    <row r="679" ht="15.75" customHeight="1"/>
-    <row r="680" ht="15.75" customHeight="1"/>
-    <row r="681" ht="15.75" customHeight="1"/>
-    <row r="682" ht="15.75" customHeight="1"/>
-    <row r="683" ht="15.75" customHeight="1"/>
-    <row r="684" ht="15.75" customHeight="1"/>
-    <row r="685" ht="15.75" customHeight="1"/>
-    <row r="686" ht="15.75" customHeight="1"/>
-    <row r="687" ht="15.75" customHeight="1"/>
-    <row r="688" ht="15.75" customHeight="1"/>
-    <row r="689" ht="15.75" customHeight="1"/>
-    <row r="690" ht="15.75" customHeight="1"/>
-    <row r="691" ht="15.75" customHeight="1"/>
-    <row r="692" ht="15.75" customHeight="1"/>
-    <row r="693" ht="15.75" customHeight="1"/>
-    <row r="694" ht="15.75" customHeight="1"/>
-    <row r="695" ht="15.75" customHeight="1"/>
-    <row r="696" ht="15.75" customHeight="1"/>
-    <row r="697" ht="15.75" customHeight="1"/>
-    <row r="698" ht="15.75" customHeight="1"/>
-    <row r="699" ht="15.75" customHeight="1"/>
-    <row r="700" ht="15.75" customHeight="1"/>
-    <row r="701" ht="15.75" customHeight="1"/>
-    <row r="702" ht="15.75" customHeight="1"/>
-    <row r="703" ht="15.75" customHeight="1"/>
-    <row r="704" ht="15.75" customHeight="1"/>
-    <row r="705" ht="15.75" customHeight="1"/>
-    <row r="706" ht="15.75" customHeight="1"/>
-    <row r="707" ht="15.75" customHeight="1"/>
-    <row r="708" ht="15.75" customHeight="1"/>
-    <row r="709" ht="15.75" customHeight="1"/>
-    <row r="710" ht="15.75" customHeight="1"/>
-    <row r="711" ht="15.75" customHeight="1"/>
-    <row r="712" ht="15.75" customHeight="1"/>
-    <row r="713" ht="15.75" customHeight="1"/>
-    <row r="714" ht="15.75" customHeight="1"/>
-    <row r="715" ht="15.75" customHeight="1"/>
-    <row r="716" ht="15.75" customHeight="1"/>
-    <row r="717" ht="15.75" customHeight="1"/>
-    <row r="718" ht="15.75" customHeight="1"/>
-    <row r="719" ht="15.75" customHeight="1"/>
-    <row r="720" ht="15.75" customHeight="1"/>
-    <row r="721" ht="15.75" customHeight="1"/>
-    <row r="722" ht="15.75" customHeight="1"/>
-    <row r="723" ht="15.75" customHeight="1"/>
-    <row r="724" ht="15.75" customHeight="1"/>
-    <row r="725" ht="15.75" customHeight="1"/>
-    <row r="726" ht="15.75" customHeight="1"/>
-    <row r="727" ht="15.75" customHeight="1"/>
-    <row r="728" ht="15.75" customHeight="1"/>
-    <row r="729" ht="15.75" customHeight="1"/>
-    <row r="730" ht="15.75" customHeight="1"/>
-    <row r="731" ht="15.75" customHeight="1"/>
-    <row r="732" ht="15.75" customHeight="1"/>
-    <row r="733" ht="15.75" customHeight="1"/>
-    <row r="734" ht="15.75" customHeight="1"/>
-    <row r="735" ht="15.75" customHeight="1"/>
-    <row r="736" ht="15.75" customHeight="1"/>
-    <row r="737" ht="15.75" customHeight="1"/>
-    <row r="738" ht="15.75" customHeight="1"/>
-    <row r="739" ht="15.75" customHeight="1"/>
-    <row r="740" ht="15.75" customHeight="1"/>
-    <row r="741" ht="15.75" customHeight="1"/>
-    <row r="742" ht="15.75" customHeight="1"/>
-    <row r="743" ht="15.75" customHeight="1"/>
-    <row r="744" ht="15.75" customHeight="1"/>
-    <row r="745" ht="15.75" customHeight="1"/>
-    <row r="746" ht="15.75" customHeight="1"/>
-    <row r="747" ht="15.75" customHeight="1"/>
-    <row r="748" ht="15.75" customHeight="1"/>
-    <row r="749" ht="15.75" customHeight="1"/>
-    <row r="750" ht="15.75" customHeight="1"/>
-    <row r="751" ht="15.75" customHeight="1"/>
-    <row r="752" ht="15.75" customHeight="1"/>
-    <row r="753" ht="15.75" customHeight="1"/>
-    <row r="754" ht="15.75" customHeight="1"/>
-    <row r="755" ht="15.75" customHeight="1"/>
-    <row r="756" ht="15.75" customHeight="1"/>
-    <row r="757" ht="15.75" customHeight="1"/>
-    <row r="758" ht="15.75" customHeight="1"/>
-    <row r="759" ht="15.75" customHeight="1"/>
-    <row r="760" ht="15.75" customHeight="1"/>
-    <row r="761" ht="15.75" customHeight="1"/>
-    <row r="762" ht="15.75" customHeight="1"/>
-    <row r="763" ht="15.75" customHeight="1"/>
-    <row r="764" ht="15.75" customHeight="1"/>
-    <row r="765" ht="15.75" customHeight="1"/>
-    <row r="766" ht="15.75" customHeight="1"/>
-    <row r="767" ht="15.75" customHeight="1"/>
-    <row r="768" ht="15.75" customHeight="1"/>
-    <row r="769" ht="15.75" customHeight="1"/>
-    <row r="770" ht="15.75" customHeight="1"/>
-    <row r="771" ht="15.75" customHeight="1"/>
-    <row r="772" ht="15.75" customHeight="1"/>
-    <row r="773" ht="15.75" customHeight="1"/>
-    <row r="774" ht="15.75" customHeight="1"/>
-    <row r="775" ht="15.75" customHeight="1"/>
-    <row r="776" ht="15.75" customHeight="1"/>
-    <row r="777" ht="15.75" customHeight="1"/>
-    <row r="778" ht="15.75" customHeight="1"/>
-    <row r="779" ht="15.75" customHeight="1"/>
-    <row r="780" ht="15.75" customHeight="1"/>
-    <row r="781" ht="15.75" customHeight="1"/>
-    <row r="782" ht="15.75" customHeight="1"/>
-    <row r="783" ht="15.75" customHeight="1"/>
-    <row r="784" ht="15.75" customHeight="1"/>
-    <row r="785" ht="15.75" customHeight="1"/>
-    <row r="786" ht="15.75" customHeight="1"/>
-    <row r="787" ht="15.75" customHeight="1"/>
-    <row r="788" ht="15.75" customHeight="1"/>
-    <row r="789" ht="15.75" customHeight="1"/>
-    <row r="790" ht="15.75" customHeight="1"/>
-    <row r="791" ht="15.75" customHeight="1"/>
-    <row r="792" ht="15.75" customHeight="1"/>
-    <row r="793" ht="15.75" customHeight="1"/>
-    <row r="794" ht="15.75" customHeight="1"/>
-    <row r="795" ht="15.75" customHeight="1"/>
-    <row r="796" ht="15.75" customHeight="1"/>
-    <row r="797" ht="15.75" customHeight="1"/>
-    <row r="798" ht="15.75" customHeight="1"/>
-    <row r="799" ht="15.75" customHeight="1"/>
-    <row r="800" ht="15.75" customHeight="1"/>
-    <row r="801" ht="15.75" customHeight="1"/>
-    <row r="802" ht="15.75" customHeight="1"/>
-    <row r="803" ht="15.75" customHeight="1"/>
-    <row r="804" ht="15.75" customHeight="1"/>
-    <row r="805" ht="15.75" customHeight="1"/>
-    <row r="806" ht="15.75" customHeight="1"/>
-    <row r="807" ht="15.75" customHeight="1"/>
-    <row r="808" ht="15.75" customHeight="1"/>
-    <row r="809" ht="15.75" customHeight="1"/>
-    <row r="810" ht="15.75" customHeight="1"/>
-    <row r="811" ht="15.75" customHeight="1"/>
-    <row r="812" ht="15.75" customHeight="1"/>
-    <row r="813" ht="15.75" customHeight="1"/>
-    <row r="814" ht="15.75" customHeight="1"/>
-    <row r="815" ht="15.75" customHeight="1"/>
-    <row r="816" ht="15.75" customHeight="1"/>
-    <row r="817" ht="15.75" customHeight="1"/>
-    <row r="818" ht="15.75" customHeight="1"/>
-    <row r="819" ht="15.75" customHeight="1"/>
-    <row r="820" ht="15.75" customHeight="1"/>
-    <row r="821" ht="15.75" customHeight="1"/>
-    <row r="822" ht="15.75" customHeight="1"/>
-    <row r="823" ht="15.75" customHeight="1"/>
-    <row r="824" ht="15.75" customHeight="1"/>
-    <row r="825" ht="15.75" customHeight="1"/>
-    <row r="826" ht="15.75" customHeight="1"/>
-    <row r="827" ht="15.75" customHeight="1"/>
-    <row r="828" ht="15.75" customHeight="1"/>
-    <row r="829" ht="15.75" customHeight="1"/>
-    <row r="830" ht="15.75" customHeight="1"/>
-    <row r="831" ht="15.75" customHeight="1"/>
-    <row r="832" ht="15.75" customHeight="1"/>
-    <row r="833" ht="15.75" customHeight="1"/>
-    <row r="834" ht="15.75" customHeight="1"/>
-    <row r="835" ht="15.75" customHeight="1"/>
-    <row r="836" ht="15.75" customHeight="1"/>
-    <row r="837" ht="15.75" customHeight="1"/>
-    <row r="838" ht="15.75" customHeight="1"/>
-    <row r="839" ht="15.75" customHeight="1"/>
-    <row r="840" ht="15.75" customHeight="1"/>
-    <row r="841" ht="15.75" customHeight="1"/>
-    <row r="842" ht="15.75" customHeight="1"/>
-    <row r="843" ht="15.75" customHeight="1"/>
-    <row r="844" ht="15.75" customHeight="1"/>
-    <row r="845" ht="15.75" customHeight="1"/>
-    <row r="846" ht="15.75" customHeight="1"/>
-    <row r="847" ht="15.75" customHeight="1"/>
-    <row r="848" ht="15.75" customHeight="1"/>
-    <row r="849" ht="15.75" customHeight="1"/>
-    <row r="850" ht="15.75" customHeight="1"/>
-    <row r="851" ht="15.75" customHeight="1"/>
-    <row r="852" ht="15.75" customHeight="1"/>
-    <row r="853" ht="15.75" customHeight="1"/>
-    <row r="854" ht="15.75" customHeight="1"/>
-    <row r="855" ht="15.75" customHeight="1"/>
-    <row r="856" ht="15.75" customHeight="1"/>
-    <row r="857" ht="15.75" customHeight="1"/>
-    <row r="858" ht="15.75" customHeight="1"/>
-    <row r="859" ht="15.75" customHeight="1"/>
-    <row r="860" ht="15.75" customHeight="1"/>
-    <row r="861" ht="15.75" customHeight="1"/>
-    <row r="862" ht="15.75" customHeight="1"/>
-    <row r="863" ht="15.75" customHeight="1"/>
-    <row r="864" ht="15.75" customHeight="1"/>
-    <row r="865" ht="15.75" customHeight="1"/>
-    <row r="866" ht="15.75" customHeight="1"/>
-    <row r="867" ht="15.75" customHeight="1"/>
-    <row r="868" ht="15.75" customHeight="1"/>
-    <row r="869" ht="15.75" customHeight="1"/>
-    <row r="870" ht="15.75" customHeight="1"/>
-    <row r="871" ht="15.75" customHeight="1"/>
-    <row r="872" ht="15.75" customHeight="1"/>
-    <row r="873" ht="15.75" customHeight="1"/>
-    <row r="874" ht="15.75" customHeight="1"/>
-    <row r="875" ht="15.75" customHeight="1"/>
-    <row r="876" ht="15.75" customHeight="1"/>
-    <row r="877" ht="15.75" customHeight="1"/>
-    <row r="878" ht="15.75" customHeight="1"/>
-    <row r="879" ht="15.75" customHeight="1"/>
-    <row r="880" ht="15.75" customHeight="1"/>
-    <row r="881" ht="15.75" customHeight="1"/>
-    <row r="882" ht="15.75" customHeight="1"/>
-    <row r="883" ht="15.75" customHeight="1"/>
-    <row r="884" ht="15.75" customHeight="1"/>
-    <row r="885" ht="15.75" customHeight="1"/>
-    <row r="886" ht="15.75" customHeight="1"/>
-    <row r="887" ht="15.75" customHeight="1"/>
-    <row r="888" ht="15.75" customHeight="1"/>
-    <row r="889" ht="15.75" customHeight="1"/>
-    <row r="890" ht="15.75" customHeight="1"/>
-    <row r="891" ht="15.75" customHeight="1"/>
-    <row r="892" ht="15.75" customHeight="1"/>
-    <row r="893" ht="15.75" customHeight="1"/>
-    <row r="894" ht="15.75" customHeight="1"/>
-    <row r="895" ht="15.75" customHeight="1"/>
-    <row r="896" ht="15.75" customHeight="1"/>
-    <row r="897" ht="15.75" customHeight="1"/>
-    <row r="898" ht="15.75" customHeight="1"/>
-    <row r="899" ht="15.75" customHeight="1"/>
-    <row r="900" ht="15.75" customHeight="1"/>
-    <row r="901" ht="15.75" customHeight="1"/>
-    <row r="902" ht="15.75" customHeight="1"/>
-    <row r="903" ht="15.75" customHeight="1"/>
-    <row r="904" ht="15.75" customHeight="1"/>
-    <row r="905" ht="15.75" customHeight="1"/>
-    <row r="906" ht="15.75" customHeight="1"/>
-    <row r="907" ht="15.75" customHeight="1"/>
-    <row r="908" ht="15.75" customHeight="1"/>
-    <row r="909" ht="15.75" customHeight="1"/>
-    <row r="910" ht="15.75" customHeight="1"/>
-    <row r="911" ht="15.75" customHeight="1"/>
-    <row r="912" ht="15.75" customHeight="1"/>
-    <row r="913" ht="15.75" customHeight="1"/>
-    <row r="914" ht="15.75" customHeight="1"/>
-    <row r="915" ht="15.75" customHeight="1"/>
-    <row r="916" ht="15.75" customHeight="1"/>
-    <row r="917" ht="15.75" customHeight="1"/>
-    <row r="918" ht="15.75" customHeight="1"/>
-    <row r="919" ht="15.75" customHeight="1"/>
-    <row r="920" ht="15.75" customHeight="1"/>
-    <row r="921" ht="15.75" customHeight="1"/>
-    <row r="922" ht="15.75" customHeight="1"/>
-    <row r="923" ht="15.75" customHeight="1"/>
-    <row r="924" ht="15.75" customHeight="1"/>
-    <row r="925" ht="15.75" customHeight="1"/>
-    <row r="926" ht="15.75" customHeight="1"/>
-    <row r="927" ht="15.75" customHeight="1"/>
-    <row r="928" ht="15.75" customHeight="1"/>
-    <row r="929" ht="15.75" customHeight="1"/>
-    <row r="930" ht="15.75" customHeight="1"/>
-    <row r="931" ht="15.75" customHeight="1"/>
-    <row r="932" ht="15.75" customHeight="1"/>
-    <row r="933" ht="15.75" customHeight="1"/>
-    <row r="934" ht="15.75" customHeight="1"/>
-    <row r="935" ht="15.75" customHeight="1"/>
-    <row r="936" ht="15.75" customHeight="1"/>
-    <row r="937" ht="15.75" customHeight="1"/>
-    <row r="938" ht="15.75" customHeight="1"/>
-    <row r="939" ht="15.75" customHeight="1"/>
-    <row r="940" ht="15.75" customHeight="1"/>
-    <row r="941" ht="15.75" customHeight="1"/>
-    <row r="942" ht="15.75" customHeight="1"/>
-    <row r="943" ht="15.75" customHeight="1"/>
-    <row r="944" ht="15.75" customHeight="1"/>
-    <row r="945" ht="15.75" customHeight="1"/>
-    <row r="946" ht="15.75" customHeight="1"/>
-    <row r="947" ht="15.75" customHeight="1"/>
-    <row r="948" ht="15.75" customHeight="1"/>
-    <row r="949" ht="15.75" customHeight="1"/>
-    <row r="950" ht="15.75" customHeight="1"/>
-    <row r="951" ht="15.75" customHeight="1"/>
-    <row r="952" ht="15.75" customHeight="1"/>
-    <row r="953" ht="15.75" customHeight="1"/>
-    <row r="954" ht="15.75" customHeight="1"/>
-    <row r="955" ht="15.75" customHeight="1"/>
-    <row r="956" ht="15.75" customHeight="1"/>
-    <row r="957" ht="15.75" customHeight="1"/>
-    <row r="958" ht="15.75" customHeight="1"/>
-    <row r="959" ht="15.75" customHeight="1"/>
-    <row r="960" ht="15.75" customHeight="1"/>
-    <row r="961" ht="15.75" customHeight="1"/>
-    <row r="962" ht="15.75" customHeight="1"/>
-    <row r="963" ht="15.75" customHeight="1"/>
-    <row r="964" ht="15.75" customHeight="1"/>
-    <row r="965" ht="15.75" customHeight="1"/>
-    <row r="966" ht="15.75" customHeight="1"/>
-    <row r="967" ht="15.75" customHeight="1"/>
-    <row r="968" ht="15.75" customHeight="1"/>
-    <row r="969" ht="15.75" customHeight="1"/>
-    <row r="970" ht="15.75" customHeight="1"/>
-    <row r="971" ht="15.75" customHeight="1"/>
-    <row r="972" ht="15.75" customHeight="1"/>
-    <row r="973" ht="15.75" customHeight="1"/>
-    <row r="974" ht="15.75" customHeight="1"/>
-    <row r="975" ht="15.75" customHeight="1"/>
-    <row r="976" ht="15.75" customHeight="1"/>
-    <row r="977" ht="15.75" customHeight="1"/>
-    <row r="978" ht="15.75" customHeight="1"/>
-    <row r="979" ht="15.75" customHeight="1"/>
-    <row r="980" ht="15.75" customHeight="1"/>
-    <row r="981" ht="15.75" customHeight="1"/>
-    <row r="982" ht="15.75" customHeight="1"/>
-    <row r="983" ht="15.75" customHeight="1"/>
-    <row r="984" ht="15.75" customHeight="1"/>
-    <row r="985" ht="15.75" customHeight="1"/>
-    <row r="986" ht="15.75" customHeight="1"/>
-    <row r="987" ht="15.75" customHeight="1"/>
-    <row r="988" ht="15.75" customHeight="1"/>
-    <row r="989" ht="15.75" customHeight="1"/>
-    <row r="990" ht="15.75" customHeight="1"/>
-    <row r="991" ht="15.75" customHeight="1"/>
-    <row r="992" ht="15.75" customHeight="1"/>
-    <row r="993" ht="15.75" customHeight="1"/>
-    <row r="994" ht="15.75" customHeight="1"/>
-    <row r="995" ht="15.75" customHeight="1"/>
-    <row r="996" ht="15.75" customHeight="1"/>
-    <row r="997" ht="15.75" customHeight="1"/>
-    <row r="998" ht="15.75" customHeight="1"/>
-    <row r="999" ht="15.75" customHeight="1"/>
-    <row r="1000" ht="15.75" customHeight="1"/>
+      <c r="G14" s="51"/>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
+      <c r="G15" s="51"/>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
+      <c r="G16" s="51"/>
+    </row>
+    <row r="17" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G17" s="51"/>
+    </row>
+    <row r="18" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G18" s="51"/>
+    </row>
+    <row r="19" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G19" s="51"/>
+    </row>
+    <row r="20" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G20" s="51"/>
+    </row>
+    <row r="21" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G21" s="51"/>
+    </row>
+    <row r="22" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G22" s="51"/>
+    </row>
+    <row r="23" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G23" s="51"/>
+    </row>
+    <row r="24" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G24" s="51"/>
+    </row>
+    <row r="25" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G25" s="51"/>
+    </row>
+    <row r="26" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G26" s="51"/>
+    </row>
+    <row r="27" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G27" s="51"/>
+    </row>
+    <row r="28" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G28" s="51"/>
+    </row>
+    <row r="29" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G29" s="51"/>
+    </row>
+    <row r="30" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G30" s="51"/>
+    </row>
+    <row r="31" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G31" s="51"/>
+    </row>
+    <row r="32" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G32" s="51"/>
+    </row>
+    <row r="33" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G33" s="51"/>
+    </row>
+    <row r="34" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G34" s="51"/>
+    </row>
+    <row r="35" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G35" s="51"/>
+    </row>
+    <row r="36" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G36" s="51"/>
+    </row>
+    <row r="37" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G37" s="51"/>
+    </row>
+    <row r="38" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G38" s="51"/>
+    </row>
+    <row r="39" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G39" s="51"/>
+    </row>
+    <row r="40" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G40" s="51"/>
+    </row>
+    <row r="41" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G41" s="51"/>
+    </row>
+    <row r="42" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G42" s="51"/>
+    </row>
+    <row r="43" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G43" s="51"/>
+    </row>
+    <row r="44" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G44" s="51"/>
+    </row>
+    <row r="45" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G45" s="51"/>
+    </row>
+    <row r="46" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G46" s="51"/>
+    </row>
+    <row r="47" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G47" s="51"/>
+    </row>
+    <row r="48" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G48" s="51"/>
+    </row>
+    <row r="49" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G49" s="51"/>
+    </row>
+    <row r="50" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G50" s="51"/>
+    </row>
+    <row r="51" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G51" s="51"/>
+    </row>
+    <row r="52" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G52" s="51"/>
+    </row>
+    <row r="53" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G53" s="51"/>
+    </row>
+    <row r="54" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G54" s="51"/>
+    </row>
+    <row r="55" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G55" s="51"/>
+    </row>
+    <row r="56" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G56" s="51"/>
+    </row>
+    <row r="57" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G57" s="51"/>
+    </row>
+    <row r="58" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G58" s="51"/>
+    </row>
+    <row r="59" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G59" s="51"/>
+    </row>
+    <row r="60" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G60" s="51"/>
+    </row>
+    <row r="61" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G61" s="51"/>
+    </row>
+    <row r="62" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G62" s="51"/>
+    </row>
+    <row r="63" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G63" s="51"/>
+    </row>
+    <row r="64" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G64" s="51"/>
+    </row>
+    <row r="65" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G65" s="51"/>
+    </row>
+    <row r="66" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G66" s="51"/>
+    </row>
+    <row r="67" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G67" s="51"/>
+    </row>
+    <row r="68" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G68" s="51"/>
+    </row>
+    <row r="69" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G69" s="51"/>
+    </row>
+    <row r="70" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G70" s="51"/>
+    </row>
+    <row r="71" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G71" s="51"/>
+    </row>
+    <row r="72" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G72" s="51"/>
+    </row>
+    <row r="73" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G73" s="51"/>
+    </row>
+    <row r="74" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G74" s="51"/>
+    </row>
+    <row r="75" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G75" s="51"/>
+    </row>
+    <row r="76" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G76" s="51"/>
+    </row>
+    <row r="77" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G77" s="51"/>
+    </row>
+    <row r="78" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G78" s="51"/>
+    </row>
+    <row r="79" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G79" s="51"/>
+    </row>
+    <row r="80" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G80" s="51"/>
+    </row>
+    <row r="81" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G81" s="51"/>
+    </row>
+    <row r="82" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G82" s="51"/>
+    </row>
+    <row r="83" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G83" s="51"/>
+    </row>
+    <row r="84" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G84" s="51"/>
+    </row>
+    <row r="85" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G85" s="51"/>
+    </row>
+    <row r="86" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G86" s="51"/>
+    </row>
+    <row r="87" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G87" s="51"/>
+    </row>
+    <row r="88" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G88" s="51"/>
+    </row>
+    <row r="89" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G89" s="51"/>
+    </row>
+    <row r="90" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G90" s="51"/>
+    </row>
+    <row r="91" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G91" s="51"/>
+    </row>
+    <row r="92" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G92" s="51"/>
+    </row>
+    <row r="93" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G93" s="51"/>
+    </row>
+    <row r="94" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G94" s="51"/>
+    </row>
+    <row r="95" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G95" s="51"/>
+    </row>
+    <row r="96" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G96" s="51"/>
+    </row>
+    <row r="97" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G97" s="51"/>
+    </row>
+    <row r="98" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G98" s="51"/>
+    </row>
+    <row r="99" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G99" s="51"/>
+    </row>
+    <row r="100" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G100" s="51"/>
+    </row>
+    <row r="101" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G101" s="51"/>
+    </row>
+    <row r="102" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G102" s="51"/>
+    </row>
+    <row r="103" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G103" s="51"/>
+    </row>
+    <row r="104" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G104" s="51"/>
+    </row>
+    <row r="105" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G105" s="51"/>
+    </row>
+    <row r="106" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G106" s="51"/>
+    </row>
+    <row r="107" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G107" s="51"/>
+    </row>
+    <row r="108" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G108" s="51"/>
+    </row>
+    <row r="109" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G109" s="51"/>
+    </row>
+    <row r="110" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G110" s="51"/>
+    </row>
+    <row r="111" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G111" s="51"/>
+    </row>
+    <row r="112" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G112" s="51"/>
+    </row>
+    <row r="113" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G113" s="51"/>
+    </row>
+    <row r="114" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G114" s="51"/>
+    </row>
+    <row r="115" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G115" s="51"/>
+    </row>
+    <row r="116" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G116" s="51"/>
+    </row>
+    <row r="117" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G117" s="51"/>
+    </row>
+    <row r="118" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G118" s="51"/>
+    </row>
+    <row r="119" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G119" s="51"/>
+    </row>
+    <row r="120" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G120" s="51"/>
+    </row>
+    <row r="121" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G121" s="51"/>
+    </row>
+    <row r="122" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G122" s="51"/>
+    </row>
+    <row r="123" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G123" s="51"/>
+    </row>
+    <row r="124" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G124" s="51"/>
+    </row>
+    <row r="125" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G125" s="51"/>
+    </row>
+    <row r="126" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G126" s="51"/>
+    </row>
+    <row r="127" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G127" s="51"/>
+    </row>
+    <row r="128" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G128" s="51"/>
+    </row>
+    <row r="129" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G129" s="51"/>
+    </row>
+    <row r="130" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G130" s="51"/>
+    </row>
+    <row r="131" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G131" s="51"/>
+    </row>
+    <row r="132" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G132" s="51"/>
+    </row>
+    <row r="133" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G133" s="51"/>
+    </row>
+    <row r="134" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G134" s="51"/>
+    </row>
+    <row r="135" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G135" s="51"/>
+    </row>
+    <row r="136" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G136" s="51"/>
+    </row>
+    <row r="137" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G137" s="51"/>
+    </row>
+    <row r="138" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G138" s="51"/>
+    </row>
+    <row r="139" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G139" s="51"/>
+    </row>
+    <row r="140" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G140" s="51"/>
+    </row>
+    <row r="141" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G141" s="51"/>
+    </row>
+    <row r="142" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G142" s="51"/>
+    </row>
+    <row r="143" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G143" s="51"/>
+    </row>
+    <row r="144" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G144" s="51"/>
+    </row>
+    <row r="145" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G145" s="51"/>
+    </row>
+    <row r="146" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G146" s="51"/>
+    </row>
+    <row r="147" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G147" s="51"/>
+    </row>
+    <row r="148" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G148" s="51"/>
+    </row>
+    <row r="149" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G149" s="51"/>
+    </row>
+    <row r="150" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G150" s="51"/>
+    </row>
+    <row r="151" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G151" s="51"/>
+    </row>
+    <row r="152" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G152" s="51"/>
+    </row>
+    <row r="153" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G153" s="51"/>
+    </row>
+    <row r="154" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G154" s="51"/>
+    </row>
+    <row r="155" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G155" s="51"/>
+    </row>
+    <row r="156" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G156" s="51"/>
+    </row>
+    <row r="157" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G157" s="51"/>
+    </row>
+    <row r="158" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G158" s="51"/>
+    </row>
+    <row r="159" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G159" s="51"/>
+    </row>
+    <row r="160" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G160" s="51"/>
+    </row>
+    <row r="161" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G161" s="51"/>
+    </row>
+    <row r="162" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G162" s="51"/>
+    </row>
+    <row r="163" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G163" s="51"/>
+    </row>
+    <row r="164" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G164" s="51"/>
+    </row>
+    <row r="165" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G165" s="51"/>
+    </row>
+    <row r="166" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G166" s="51"/>
+    </row>
+    <row r="167" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G167" s="51"/>
+    </row>
+    <row r="168" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G168" s="51"/>
+    </row>
+    <row r="169" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G169" s="51"/>
+    </row>
+    <row r="170" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G170" s="51"/>
+    </row>
+    <row r="171" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G171" s="51"/>
+    </row>
+    <row r="172" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G172" s="51"/>
+    </row>
+    <row r="173" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G173" s="51"/>
+    </row>
+    <row r="174" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G174" s="51"/>
+    </row>
+    <row r="175" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G175" s="51"/>
+    </row>
+    <row r="176" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G176" s="51"/>
+    </row>
+    <row r="177" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G177" s="51"/>
+    </row>
+    <row r="178" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G178" s="51"/>
+    </row>
+    <row r="179" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G179" s="51"/>
+    </row>
+    <row r="180" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G180" s="51"/>
+    </row>
+    <row r="181" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G181" s="51"/>
+    </row>
+    <row r="182" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G182" s="51"/>
+    </row>
+    <row r="183" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G183" s="51"/>
+    </row>
+    <row r="184" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G184" s="51"/>
+    </row>
+    <row r="185" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G185" s="51"/>
+    </row>
+    <row r="186" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G186" s="51"/>
+    </row>
+    <row r="187" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G187" s="51"/>
+    </row>
+    <row r="188" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G188" s="51"/>
+    </row>
+    <row r="189" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G189" s="51"/>
+    </row>
+    <row r="190" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G190" s="51"/>
+    </row>
+    <row r="191" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G191" s="51"/>
+    </row>
+    <row r="192" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G192" s="51"/>
+    </row>
+    <row r="193" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G193" s="51"/>
+    </row>
+    <row r="194" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G194" s="51"/>
+    </row>
+    <row r="195" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G195" s="51"/>
+    </row>
+    <row r="196" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G196" s="51"/>
+    </row>
+    <row r="197" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G197" s="51"/>
+    </row>
+    <row r="198" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G198" s="51"/>
+    </row>
+    <row r="199" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G199" s="51"/>
+    </row>
+    <row r="200" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G200" s="51"/>
+    </row>
+    <row r="201" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G201" s="51"/>
+    </row>
+    <row r="202" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G202" s="51"/>
+    </row>
+    <row r="203" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G203" s="51"/>
+    </row>
+    <row r="204" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G204" s="51"/>
+    </row>
+    <row r="205" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G205" s="51"/>
+    </row>
+    <row r="206" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G206" s="51"/>
+    </row>
+    <row r="207" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G207" s="51"/>
+    </row>
+    <row r="208" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G208" s="51"/>
+    </row>
+    <row r="209" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G209" s="51"/>
+    </row>
+    <row r="210" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G210" s="51"/>
+    </row>
+    <row r="211" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G211" s="51"/>
+    </row>
+    <row r="212" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G212" s="51"/>
+    </row>
+    <row r="213" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G213" s="51"/>
+    </row>
+    <row r="214" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G214" s="51"/>
+    </row>
+    <row r="215" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G215" s="51"/>
+    </row>
+    <row r="216" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G216" s="51"/>
+    </row>
+    <row r="217" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G217" s="51"/>
+    </row>
+    <row r="218" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G218" s="51"/>
+    </row>
+    <row r="219" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G219" s="51"/>
+    </row>
+    <row r="220" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G220" s="51"/>
+    </row>
+    <row r="221" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G221" s="51"/>
+    </row>
+    <row r="222" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G222" s="51"/>
+    </row>
+    <row r="223" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G223" s="51"/>
+    </row>
+    <row r="224" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G224" s="51"/>
+    </row>
+    <row r="225" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G225" s="51"/>
+    </row>
+    <row r="226" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G226" s="51"/>
+    </row>
+    <row r="227" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G227" s="51"/>
+    </row>
+    <row r="228" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G228" s="51"/>
+    </row>
+    <row r="229" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G229" s="51"/>
+    </row>
+    <row r="230" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G230" s="51"/>
+    </row>
+    <row r="231" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G231" s="51"/>
+    </row>
+    <row r="232" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G232" s="51"/>
+    </row>
+    <row r="233" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G233" s="51"/>
+    </row>
+    <row r="234" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G234" s="51"/>
+    </row>
+    <row r="235" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G235" s="51"/>
+    </row>
+    <row r="236" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G236" s="51"/>
+    </row>
+    <row r="237" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G237" s="51"/>
+    </row>
+    <row r="238" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G238" s="51"/>
+    </row>
+    <row r="239" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G239" s="51"/>
+    </row>
+    <row r="240" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G240" s="51"/>
+    </row>
+    <row r="241" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G241" s="51"/>
+    </row>
+    <row r="242" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G242" s="51"/>
+    </row>
+    <row r="243" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G243" s="51"/>
+    </row>
+    <row r="244" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G244" s="51"/>
+    </row>
+    <row r="245" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G245" s="51"/>
+    </row>
+    <row r="246" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G246" s="51"/>
+    </row>
+    <row r="247" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G247" s="51"/>
+    </row>
+    <row r="248" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G248" s="51"/>
+    </row>
+    <row r="249" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G249" s="51"/>
+    </row>
+    <row r="250" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G250" s="51"/>
+    </row>
+    <row r="251" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G251" s="51"/>
+    </row>
+    <row r="252" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G252" s="51"/>
+    </row>
+    <row r="253" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G253" s="51"/>
+    </row>
+    <row r="254" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G254" s="51"/>
+    </row>
+    <row r="255" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G255" s="51"/>
+    </row>
+    <row r="256" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G256" s="51"/>
+    </row>
+    <row r="257" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G257" s="51"/>
+    </row>
+    <row r="258" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G258" s="51"/>
+    </row>
+    <row r="259" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G259" s="51"/>
+    </row>
+    <row r="260" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G260" s="51"/>
+    </row>
+    <row r="261" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G261" s="51"/>
+    </row>
+    <row r="262" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G262" s="51"/>
+    </row>
+    <row r="263" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G263" s="51"/>
+    </row>
+    <row r="264" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G264" s="51"/>
+    </row>
+    <row r="265" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G265" s="51"/>
+    </row>
+    <row r="266" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G266" s="51"/>
+    </row>
+    <row r="267" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G267" s="51"/>
+    </row>
+    <row r="268" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G268" s="51"/>
+    </row>
+    <row r="269" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G269" s="51"/>
+    </row>
+    <row r="270" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G270" s="51"/>
+    </row>
+    <row r="271" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G271" s="51"/>
+    </row>
+    <row r="272" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G272" s="51"/>
+    </row>
+    <row r="273" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G273" s="51"/>
+    </row>
+    <row r="274" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G274" s="51"/>
+    </row>
+    <row r="275" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G275" s="51"/>
+    </row>
+    <row r="276" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G276" s="51"/>
+    </row>
+    <row r="277" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G277" s="51"/>
+    </row>
+    <row r="278" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G278" s="51"/>
+    </row>
+    <row r="279" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G279" s="51"/>
+    </row>
+    <row r="280" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G280" s="51"/>
+    </row>
+    <row r="281" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G281" s="51"/>
+    </row>
+    <row r="282" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G282" s="51"/>
+    </row>
+    <row r="283" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G283" s="51"/>
+    </row>
+    <row r="284" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G284" s="51"/>
+    </row>
+    <row r="285" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G285" s="51"/>
+    </row>
+    <row r="286" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G286" s="51"/>
+    </row>
+    <row r="287" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G287" s="51"/>
+    </row>
+    <row r="288" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G288" s="51"/>
+    </row>
+    <row r="289" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G289" s="51"/>
+    </row>
+    <row r="290" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G290" s="51"/>
+    </row>
+    <row r="291" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G291" s="51"/>
+    </row>
+    <row r="292" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G292" s="51"/>
+    </row>
+    <row r="293" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G293" s="51"/>
+    </row>
+    <row r="294" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G294" s="51"/>
+    </row>
+    <row r="295" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G295" s="51"/>
+    </row>
+    <row r="296" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G296" s="51"/>
+    </row>
+    <row r="297" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G297" s="51"/>
+    </row>
+    <row r="298" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G298" s="51"/>
+    </row>
+    <row r="299" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G299" s="51"/>
+    </row>
+    <row r="300" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G300" s="51"/>
+    </row>
+    <row r="301" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G301" s="51"/>
+    </row>
+    <row r="302" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G302" s="51"/>
+    </row>
+    <row r="303" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G303" s="51"/>
+    </row>
+    <row r="304" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G304" s="51"/>
+    </row>
+    <row r="305" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G305" s="51"/>
+    </row>
+    <row r="306" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G306" s="51"/>
+    </row>
+    <row r="307" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G307" s="51"/>
+    </row>
+    <row r="308" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G308" s="51"/>
+    </row>
+    <row r="309" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G309" s="51"/>
+    </row>
+    <row r="310" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G310" s="51"/>
+    </row>
+    <row r="311" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G311" s="51"/>
+    </row>
+    <row r="312" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G312" s="51"/>
+    </row>
+    <row r="313" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G313" s="51"/>
+    </row>
+    <row r="314" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G314" s="51"/>
+    </row>
+    <row r="315" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G315" s="51"/>
+    </row>
+    <row r="316" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G316" s="51"/>
+    </row>
+    <row r="317" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G317" s="51"/>
+    </row>
+    <row r="318" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G318" s="51"/>
+    </row>
+    <row r="319" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G319" s="51"/>
+    </row>
+    <row r="320" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G320" s="51"/>
+    </row>
+    <row r="321" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G321" s="51"/>
+    </row>
+    <row r="322" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G322" s="51"/>
+    </row>
+    <row r="323" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G323" s="51"/>
+    </row>
+    <row r="324" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G324" s="51"/>
+    </row>
+    <row r="325" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G325" s="51"/>
+    </row>
+    <row r="326" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G326" s="51"/>
+    </row>
+    <row r="327" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G327" s="51"/>
+    </row>
+    <row r="328" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G328" s="51"/>
+    </row>
+    <row r="329" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G329" s="51"/>
+    </row>
+    <row r="330" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G330" s="51"/>
+    </row>
+    <row r="331" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G331" s="51"/>
+    </row>
+    <row r="332" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G332" s="51"/>
+    </row>
+    <row r="333" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G333" s="51"/>
+    </row>
+    <row r="334" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G334" s="51"/>
+    </row>
+    <row r="335" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G335" s="51"/>
+    </row>
+    <row r="336" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G336" s="51"/>
+    </row>
+    <row r="337" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G337" s="51"/>
+    </row>
+    <row r="338" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G338" s="51"/>
+    </row>
+    <row r="339" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G339" s="51"/>
+    </row>
+    <row r="340" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G340" s="51"/>
+    </row>
+    <row r="341" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G341" s="51"/>
+    </row>
+    <row r="342" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G342" s="51"/>
+    </row>
+    <row r="343" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G343" s="51"/>
+    </row>
+    <row r="344" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G344" s="51"/>
+    </row>
+    <row r="345" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G345" s="51"/>
+    </row>
+    <row r="346" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G346" s="51"/>
+    </row>
+    <row r="347" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G347" s="51"/>
+    </row>
+    <row r="348" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G348" s="51"/>
+    </row>
+    <row r="349" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G349" s="51"/>
+    </row>
+    <row r="350" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G350" s="51"/>
+    </row>
+    <row r="351" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G351" s="51"/>
+    </row>
+    <row r="352" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G352" s="51"/>
+    </row>
+    <row r="353" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G353" s="51"/>
+    </row>
+    <row r="354" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G354" s="51"/>
+    </row>
+    <row r="355" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G355" s="51"/>
+    </row>
+    <row r="356" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G356" s="51"/>
+    </row>
+    <row r="357" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G357" s="51"/>
+    </row>
+    <row r="358" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G358" s="51"/>
+    </row>
+    <row r="359" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G359" s="51"/>
+    </row>
+    <row r="360" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G360" s="51"/>
+    </row>
+    <row r="361" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G361" s="51"/>
+    </row>
+    <row r="362" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G362" s="51"/>
+    </row>
+    <row r="363" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G363" s="51"/>
+    </row>
+    <row r="364" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G364" s="51"/>
+    </row>
+    <row r="365" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G365" s="51"/>
+    </row>
+    <row r="366" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G366" s="51"/>
+    </row>
+    <row r="367" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G367" s="51"/>
+    </row>
+    <row r="368" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G368" s="51"/>
+    </row>
+    <row r="369" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G369" s="51"/>
+    </row>
+    <row r="370" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G370" s="51"/>
+    </row>
+    <row r="371" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G371" s="51"/>
+    </row>
+    <row r="372" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G372" s="51"/>
+    </row>
+    <row r="373" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G373" s="51"/>
+    </row>
+    <row r="374" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G374" s="51"/>
+    </row>
+    <row r="375" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G375" s="51"/>
+    </row>
+    <row r="376" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G376" s="51"/>
+    </row>
+    <row r="377" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G377" s="51"/>
+    </row>
+    <row r="378" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G378" s="51"/>
+    </row>
+    <row r="379" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G379" s="51"/>
+    </row>
+    <row r="380" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G380" s="51"/>
+    </row>
+    <row r="381" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G381" s="51"/>
+    </row>
+    <row r="382" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G382" s="51"/>
+    </row>
+    <row r="383" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G383" s="51"/>
+    </row>
+    <row r="384" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G384" s="51"/>
+    </row>
+    <row r="385" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G385" s="51"/>
+    </row>
+    <row r="386" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G386" s="51"/>
+    </row>
+    <row r="387" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G387" s="51"/>
+    </row>
+    <row r="388" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G388" s="51"/>
+    </row>
+    <row r="389" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G389" s="51"/>
+    </row>
+    <row r="390" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G390" s="51"/>
+    </row>
+    <row r="391" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G391" s="51"/>
+    </row>
+    <row r="392" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G392" s="51"/>
+    </row>
+    <row r="393" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G393" s="51"/>
+    </row>
+    <row r="394" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G394" s="51"/>
+    </row>
+    <row r="395" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G395" s="51"/>
+    </row>
+    <row r="396" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G396" s="51"/>
+    </row>
+    <row r="397" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G397" s="51"/>
+    </row>
+    <row r="398" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G398" s="51"/>
+    </row>
+    <row r="399" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G399" s="51"/>
+    </row>
+    <row r="400" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G400" s="51"/>
+    </row>
+    <row r="401" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G401" s="51"/>
+    </row>
+    <row r="402" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G402" s="51"/>
+    </row>
+    <row r="403" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G403" s="51"/>
+    </row>
+    <row r="404" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G404" s="51"/>
+    </row>
+    <row r="405" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G405" s="51"/>
+    </row>
+    <row r="406" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G406" s="51"/>
+    </row>
+    <row r="407" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G407" s="51"/>
+    </row>
+    <row r="408" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G408" s="51"/>
+    </row>
+    <row r="409" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G409" s="51"/>
+    </row>
+    <row r="410" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G410" s="51"/>
+    </row>
+    <row r="411" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G411" s="51"/>
+    </row>
+    <row r="412" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G412" s="51"/>
+    </row>
+    <row r="413" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G413" s="51"/>
+    </row>
+    <row r="414" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G414" s="51"/>
+    </row>
+    <row r="415" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G415" s="51"/>
+    </row>
+    <row r="416" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G416" s="51"/>
+    </row>
+    <row r="417" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G417" s="51"/>
+    </row>
+    <row r="418" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G418" s="51"/>
+    </row>
+    <row r="419" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G419" s="51"/>
+    </row>
+    <row r="420" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G420" s="51"/>
+    </row>
+    <row r="421" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G421" s="51"/>
+    </row>
+    <row r="422" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G422" s="51"/>
+    </row>
+    <row r="423" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G423" s="51"/>
+    </row>
+    <row r="424" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G424" s="51"/>
+    </row>
+    <row r="425" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G425" s="51"/>
+    </row>
+    <row r="426" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G426" s="51"/>
+    </row>
+    <row r="427" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G427" s="51"/>
+    </row>
+    <row r="428" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G428" s="51"/>
+    </row>
+    <row r="429" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G429" s="51"/>
+    </row>
+    <row r="430" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G430" s="51"/>
+    </row>
+    <row r="431" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G431" s="51"/>
+    </row>
+    <row r="432" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G432" s="51"/>
+    </row>
+    <row r="433" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G433" s="51"/>
+    </row>
+    <row r="434" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G434" s="51"/>
+    </row>
+    <row r="435" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G435" s="51"/>
+    </row>
+    <row r="436" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G436" s="51"/>
+    </row>
+    <row r="437" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G437" s="51"/>
+    </row>
+    <row r="438" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G438" s="51"/>
+    </row>
+    <row r="439" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G439" s="51"/>
+    </row>
+    <row r="440" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G440" s="51"/>
+    </row>
+    <row r="441" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G441" s="51"/>
+    </row>
+    <row r="442" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G442" s="51"/>
+    </row>
+    <row r="443" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G443" s="51"/>
+    </row>
+    <row r="444" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G444" s="51"/>
+    </row>
+    <row r="445" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G445" s="51"/>
+    </row>
+    <row r="446" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G446" s="51"/>
+    </row>
+    <row r="447" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G447" s="51"/>
+    </row>
+    <row r="448" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G448" s="51"/>
+    </row>
+    <row r="449" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G449" s="51"/>
+    </row>
+    <row r="450" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G450" s="51"/>
+    </row>
+    <row r="451" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G451" s="51"/>
+    </row>
+    <row r="452" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G452" s="51"/>
+    </row>
+    <row r="453" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G453" s="51"/>
+    </row>
+    <row r="454" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G454" s="51"/>
+    </row>
+    <row r="455" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G455" s="51"/>
+    </row>
+    <row r="456" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G456" s="51"/>
+    </row>
+    <row r="457" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G457" s="51"/>
+    </row>
+    <row r="458" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G458" s="51"/>
+    </row>
+    <row r="459" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G459" s="51"/>
+    </row>
+    <row r="460" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G460" s="51"/>
+    </row>
+    <row r="461" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G461" s="51"/>
+    </row>
+    <row r="462" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G462" s="51"/>
+    </row>
+    <row r="463" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G463" s="51"/>
+    </row>
+    <row r="464" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G464" s="51"/>
+    </row>
+    <row r="465" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G465" s="51"/>
+    </row>
+    <row r="466" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G466" s="51"/>
+    </row>
+    <row r="467" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G467" s="51"/>
+    </row>
+    <row r="468" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G468" s="51"/>
+    </row>
+    <row r="469" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G469" s="51"/>
+    </row>
+    <row r="470" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G470" s="51"/>
+    </row>
+    <row r="471" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G471" s="51"/>
+    </row>
+    <row r="472" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G472" s="51"/>
+    </row>
+    <row r="473" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G473" s="51"/>
+    </row>
+    <row r="474" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G474" s="51"/>
+    </row>
+    <row r="475" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G475" s="51"/>
+    </row>
+    <row r="476" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G476" s="51"/>
+    </row>
+    <row r="477" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G477" s="51"/>
+    </row>
+    <row r="478" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G478" s="51"/>
+    </row>
+    <row r="479" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G479" s="51"/>
+    </row>
+    <row r="480" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G480" s="51"/>
+    </row>
+    <row r="481" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G481" s="51"/>
+    </row>
+    <row r="482" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G482" s="51"/>
+    </row>
+    <row r="483" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G483" s="51"/>
+    </row>
+    <row r="484" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G484" s="51"/>
+    </row>
+    <row r="485" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G485" s="51"/>
+    </row>
+    <row r="486" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G486" s="51"/>
+    </row>
+    <row r="487" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G487" s="51"/>
+    </row>
+    <row r="488" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G488" s="51"/>
+    </row>
+    <row r="489" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G489" s="51"/>
+    </row>
+    <row r="490" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G490" s="51"/>
+    </row>
+    <row r="491" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G491" s="51"/>
+    </row>
+    <row r="492" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G492" s="51"/>
+    </row>
+    <row r="493" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G493" s="51"/>
+    </row>
+    <row r="494" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G494" s="51"/>
+    </row>
+    <row r="495" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G495" s="51"/>
+    </row>
+    <row r="496" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G496" s="51"/>
+    </row>
+    <row r="497" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G497" s="51"/>
+    </row>
+    <row r="498" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G498" s="51"/>
+    </row>
+    <row r="499" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G499" s="51"/>
+    </row>
+    <row r="500" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G500" s="51"/>
+    </row>
+    <row r="501" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G501" s="51"/>
+    </row>
+    <row r="502" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G502" s="51"/>
+    </row>
+    <row r="503" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G503" s="51"/>
+    </row>
+    <row r="504" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G504" s="51"/>
+    </row>
+    <row r="505" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G505" s="51"/>
+    </row>
+    <row r="506" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G506" s="51"/>
+    </row>
+    <row r="507" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G507" s="51"/>
+    </row>
+    <row r="508" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G508" s="51"/>
+    </row>
+    <row r="509" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G509" s="51"/>
+    </row>
+    <row r="510" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G510" s="51"/>
+    </row>
+    <row r="511" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G511" s="51"/>
+    </row>
+    <row r="512" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G512" s="51"/>
+    </row>
+    <row r="513" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G513" s="51"/>
+    </row>
+    <row r="514" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G514" s="51"/>
+    </row>
+    <row r="515" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G515" s="51"/>
+    </row>
+    <row r="516" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G516" s="51"/>
+    </row>
+    <row r="517" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G517" s="51"/>
+    </row>
+    <row r="518" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G518" s="51"/>
+    </row>
+    <row r="519" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G519" s="51"/>
+    </row>
+    <row r="520" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G520" s="51"/>
+    </row>
+    <row r="521" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G521" s="51"/>
+    </row>
+    <row r="522" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G522" s="51"/>
+    </row>
+    <row r="523" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G523" s="51"/>
+    </row>
+    <row r="524" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G524" s="51"/>
+    </row>
+    <row r="525" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G525" s="51"/>
+    </row>
+    <row r="526" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G526" s="51"/>
+    </row>
+    <row r="527" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G527" s="51"/>
+    </row>
+    <row r="528" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G528" s="51"/>
+    </row>
+    <row r="529" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G529" s="51"/>
+    </row>
+    <row r="530" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G530" s="51"/>
+    </row>
+    <row r="531" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G531" s="51"/>
+    </row>
+    <row r="532" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G532" s="51"/>
+    </row>
+    <row r="533" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G533" s="51"/>
+    </row>
+    <row r="534" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G534" s="51"/>
+    </row>
+    <row r="535" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G535" s="51"/>
+    </row>
+    <row r="536" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G536" s="51"/>
+    </row>
+    <row r="537" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G537" s="51"/>
+    </row>
+    <row r="538" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G538" s="51"/>
+    </row>
+    <row r="539" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G539" s="51"/>
+    </row>
+    <row r="540" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G540" s="51"/>
+    </row>
+    <row r="541" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G541" s="51"/>
+    </row>
+    <row r="542" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G542" s="51"/>
+    </row>
+    <row r="543" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G543" s="51"/>
+    </row>
+    <row r="544" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G544" s="51"/>
+    </row>
+    <row r="545" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G545" s="51"/>
+    </row>
+    <row r="546" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G546" s="51"/>
+    </row>
+    <row r="547" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G547" s="51"/>
+    </row>
+    <row r="548" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G548" s="51"/>
+    </row>
+    <row r="549" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G549" s="51"/>
+    </row>
+    <row r="550" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G550" s="51"/>
+    </row>
+    <row r="551" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G551" s="51"/>
+    </row>
+    <row r="552" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G552" s="51"/>
+    </row>
+    <row r="553" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G553" s="51"/>
+    </row>
+    <row r="554" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G554" s="51"/>
+    </row>
+    <row r="555" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G555" s="51"/>
+    </row>
+    <row r="556" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G556" s="51"/>
+    </row>
+    <row r="557" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G557" s="51"/>
+    </row>
+    <row r="558" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G558" s="51"/>
+    </row>
+    <row r="559" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G559" s="51"/>
+    </row>
+    <row r="560" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G560" s="51"/>
+    </row>
+    <row r="561" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G561" s="51"/>
+    </row>
+    <row r="562" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G562" s="51"/>
+    </row>
+    <row r="563" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G563" s="51"/>
+    </row>
+    <row r="564" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G564" s="51"/>
+    </row>
+    <row r="565" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G565" s="51"/>
+    </row>
+    <row r="566" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G566" s="51"/>
+    </row>
+    <row r="567" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G567" s="51"/>
+    </row>
+    <row r="568" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G568" s="51"/>
+    </row>
+    <row r="569" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G569" s="51"/>
+    </row>
+    <row r="570" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G570" s="51"/>
+    </row>
+    <row r="571" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G571" s="51"/>
+    </row>
+    <row r="572" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G572" s="51"/>
+    </row>
+    <row r="573" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G573" s="51"/>
+    </row>
+    <row r="574" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G574" s="51"/>
+    </row>
+    <row r="575" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G575" s="51"/>
+    </row>
+    <row r="576" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G576" s="51"/>
+    </row>
+    <row r="577" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G577" s="51"/>
+    </row>
+    <row r="578" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G578" s="51"/>
+    </row>
+    <row r="579" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G579" s="51"/>
+    </row>
+    <row r="580" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G580" s="51"/>
+    </row>
+    <row r="581" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G581" s="51"/>
+    </row>
+    <row r="582" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G582" s="51"/>
+    </row>
+    <row r="583" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G583" s="51"/>
+    </row>
+    <row r="584" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G584" s="51"/>
+    </row>
+    <row r="585" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G585" s="51"/>
+    </row>
+    <row r="586" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G586" s="51"/>
+    </row>
+    <row r="587" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G587" s="51"/>
+    </row>
+    <row r="588" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G588" s="51"/>
+    </row>
+    <row r="589" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G589" s="51"/>
+    </row>
+    <row r="590" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G590" s="51"/>
+    </row>
+    <row r="591" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G591" s="51"/>
+    </row>
+    <row r="592" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G592" s="51"/>
+    </row>
+    <row r="593" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G593" s="51"/>
+    </row>
+    <row r="594" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G594" s="51"/>
+    </row>
+    <row r="595" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G595" s="51"/>
+    </row>
+    <row r="596" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G596" s="51"/>
+    </row>
+    <row r="597" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G597" s="51"/>
+    </row>
+    <row r="598" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G598" s="51"/>
+    </row>
+    <row r="599" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G599" s="51"/>
+    </row>
+    <row r="600" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G600" s="51"/>
+    </row>
+    <row r="601" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G601" s="51"/>
+    </row>
+    <row r="602" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G602" s="51"/>
+    </row>
+    <row r="603" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G603" s="51"/>
+    </row>
+    <row r="604" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G604" s="51"/>
+    </row>
+    <row r="605" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G605" s="51"/>
+    </row>
+    <row r="606" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G606" s="51"/>
+    </row>
+    <row r="607" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G607" s="51"/>
+    </row>
+    <row r="608" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G608" s="51"/>
+    </row>
+    <row r="609" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G609" s="51"/>
+    </row>
+    <row r="610" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G610" s="51"/>
+    </row>
+    <row r="611" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G611" s="51"/>
+    </row>
+    <row r="612" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G612" s="51"/>
+    </row>
+    <row r="613" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G613" s="51"/>
+    </row>
+    <row r="614" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G614" s="51"/>
+    </row>
+    <row r="615" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G615" s="51"/>
+    </row>
+    <row r="616" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G616" s="51"/>
+    </row>
+    <row r="617" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G617" s="51"/>
+    </row>
+    <row r="618" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G618" s="51"/>
+    </row>
+    <row r="619" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G619" s="51"/>
+    </row>
+    <row r="620" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G620" s="51"/>
+    </row>
+    <row r="621" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G621" s="51"/>
+    </row>
+    <row r="622" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G622" s="51"/>
+    </row>
+    <row r="623" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G623" s="51"/>
+    </row>
+    <row r="624" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G624" s="51"/>
+    </row>
+    <row r="625" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G625" s="51"/>
+    </row>
+    <row r="626" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G626" s="51"/>
+    </row>
+    <row r="627" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G627" s="51"/>
+    </row>
+    <row r="628" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G628" s="51"/>
+    </row>
+    <row r="629" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G629" s="51"/>
+    </row>
+    <row r="630" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G630" s="51"/>
+    </row>
+    <row r="631" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G631" s="51"/>
+    </row>
+    <row r="632" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G632" s="51"/>
+    </row>
+    <row r="633" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G633" s="51"/>
+    </row>
+    <row r="634" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G634" s="51"/>
+    </row>
+    <row r="635" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G635" s="51"/>
+    </row>
+    <row r="636" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G636" s="51"/>
+    </row>
+    <row r="637" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G637" s="51"/>
+    </row>
+    <row r="638" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G638" s="51"/>
+    </row>
+    <row r="639" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G639" s="51"/>
+    </row>
+    <row r="640" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G640" s="51"/>
+    </row>
+    <row r="641" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G641" s="51"/>
+    </row>
+    <row r="642" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G642" s="51"/>
+    </row>
+    <row r="643" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G643" s="51"/>
+    </row>
+    <row r="644" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G644" s="51"/>
+    </row>
+    <row r="645" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G645" s="51"/>
+    </row>
+    <row r="646" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G646" s="51"/>
+    </row>
+    <row r="647" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G647" s="51"/>
+    </row>
+    <row r="648" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G648" s="51"/>
+    </row>
+    <row r="649" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G649" s="51"/>
+    </row>
+    <row r="650" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G650" s="51"/>
+    </row>
+    <row r="651" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G651" s="51"/>
+    </row>
+    <row r="652" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G652" s="51"/>
+    </row>
+    <row r="653" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G653" s="51"/>
+    </row>
+    <row r="654" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G654" s="51"/>
+    </row>
+    <row r="655" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G655" s="51"/>
+    </row>
+    <row r="656" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G656" s="51"/>
+    </row>
+    <row r="657" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G657" s="51"/>
+    </row>
+    <row r="658" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G658" s="51"/>
+    </row>
+    <row r="659" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G659" s="51"/>
+    </row>
+    <row r="660" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G660" s="51"/>
+    </row>
+    <row r="661" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G661" s="51"/>
+    </row>
+    <row r="662" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G662" s="51"/>
+    </row>
+    <row r="663" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G663" s="51"/>
+    </row>
+    <row r="664" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G664" s="51"/>
+    </row>
+    <row r="665" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G665" s="51"/>
+    </row>
+    <row r="666" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G666" s="51"/>
+    </row>
+    <row r="667" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G667" s="51"/>
+    </row>
+    <row r="668" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G668" s="51"/>
+    </row>
+    <row r="669" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G669" s="51"/>
+    </row>
+    <row r="670" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G670" s="51"/>
+    </row>
+    <row r="671" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G671" s="51"/>
+    </row>
+    <row r="672" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G672" s="51"/>
+    </row>
+    <row r="673" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G673" s="51"/>
+    </row>
+    <row r="674" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G674" s="51"/>
+    </row>
+    <row r="675" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G675" s="51"/>
+    </row>
+    <row r="676" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G676" s="51"/>
+    </row>
+    <row r="677" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G677" s="51"/>
+    </row>
+    <row r="678" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G678" s="51"/>
+    </row>
+    <row r="679" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G679" s="51"/>
+    </row>
+    <row r="680" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G680" s="51"/>
+    </row>
+    <row r="681" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G681" s="51"/>
+    </row>
+    <row r="682" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G682" s="51"/>
+    </row>
+    <row r="683" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G683" s="51"/>
+    </row>
+    <row r="684" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G684" s="51"/>
+    </row>
+    <row r="685" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G685" s="51"/>
+    </row>
+    <row r="686" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G686" s="51"/>
+    </row>
+    <row r="687" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G687" s="51"/>
+    </row>
+    <row r="688" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G688" s="51"/>
+    </row>
+    <row r="689" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G689" s="51"/>
+    </row>
+    <row r="690" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G690" s="51"/>
+    </row>
+    <row r="691" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G691" s="51"/>
+    </row>
+    <row r="692" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G692" s="51"/>
+    </row>
+    <row r="693" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G693" s="51"/>
+    </row>
+    <row r="694" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G694" s="51"/>
+    </row>
+    <row r="695" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G695" s="51"/>
+    </row>
+    <row r="696" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G696" s="51"/>
+    </row>
+    <row r="697" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G697" s="51"/>
+    </row>
+    <row r="698" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G698" s="51"/>
+    </row>
+    <row r="699" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G699" s="51"/>
+    </row>
+    <row r="700" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G700" s="51"/>
+    </row>
+    <row r="701" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G701" s="51"/>
+    </row>
+    <row r="702" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G702" s="51"/>
+    </row>
+    <row r="703" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G703" s="51"/>
+    </row>
+    <row r="704" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G704" s="51"/>
+    </row>
+    <row r="705" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G705" s="51"/>
+    </row>
+    <row r="706" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G706" s="51"/>
+    </row>
+    <row r="707" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G707" s="51"/>
+    </row>
+    <row r="708" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G708" s="51"/>
+    </row>
+    <row r="709" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G709" s="51"/>
+    </row>
+    <row r="710" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G710" s="51"/>
+    </row>
+    <row r="711" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G711" s="51"/>
+    </row>
+    <row r="712" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G712" s="51"/>
+    </row>
+    <row r="713" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G713" s="51"/>
+    </row>
+    <row r="714" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G714" s="51"/>
+    </row>
+    <row r="715" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G715" s="51"/>
+    </row>
+    <row r="716" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G716" s="51"/>
+    </row>
+    <row r="717" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G717" s="51"/>
+    </row>
+    <row r="718" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G718" s="51"/>
+    </row>
+    <row r="719" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G719" s="51"/>
+    </row>
+    <row r="720" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G720" s="51"/>
+    </row>
+    <row r="721" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G721" s="51"/>
+    </row>
+    <row r="722" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G722" s="51"/>
+    </row>
+    <row r="723" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G723" s="51"/>
+    </row>
+    <row r="724" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G724" s="51"/>
+    </row>
+    <row r="725" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G725" s="51"/>
+    </row>
+    <row r="726" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G726" s="51"/>
+    </row>
+    <row r="727" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G727" s="51"/>
+    </row>
+    <row r="728" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G728" s="51"/>
+    </row>
+    <row r="729" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G729" s="51"/>
+    </row>
+    <row r="730" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G730" s="51"/>
+    </row>
+    <row r="731" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G731" s="51"/>
+    </row>
+    <row r="732" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G732" s="51"/>
+    </row>
+    <row r="733" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G733" s="51"/>
+    </row>
+    <row r="734" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G734" s="51"/>
+    </row>
+    <row r="735" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G735" s="51"/>
+    </row>
+    <row r="736" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G736" s="51"/>
+    </row>
+    <row r="737" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G737" s="51"/>
+    </row>
+    <row r="738" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G738" s="51"/>
+    </row>
+    <row r="739" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G739" s="51"/>
+    </row>
+    <row r="740" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G740" s="51"/>
+    </row>
+    <row r="741" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G741" s="51"/>
+    </row>
+    <row r="742" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G742" s="51"/>
+    </row>
+    <row r="743" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G743" s="51"/>
+    </row>
+    <row r="744" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G744" s="51"/>
+    </row>
+    <row r="745" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G745" s="51"/>
+    </row>
+    <row r="746" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G746" s="51"/>
+    </row>
+    <row r="747" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G747" s="51"/>
+    </row>
+    <row r="748" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G748" s="51"/>
+    </row>
+    <row r="749" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G749" s="51"/>
+    </row>
+    <row r="750" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G750" s="51"/>
+    </row>
+    <row r="751" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G751" s="51"/>
+    </row>
+    <row r="752" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G752" s="51"/>
+    </row>
+    <row r="753" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G753" s="51"/>
+    </row>
+    <row r="754" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G754" s="51"/>
+    </row>
+    <row r="755" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G755" s="51"/>
+    </row>
+    <row r="756" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G756" s="51"/>
+    </row>
+    <row r="757" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G757" s="51"/>
+    </row>
+    <row r="758" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G758" s="51"/>
+    </row>
+    <row r="759" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G759" s="51"/>
+    </row>
+    <row r="760" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G760" s="51"/>
+    </row>
+    <row r="761" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G761" s="51"/>
+    </row>
+    <row r="762" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G762" s="51"/>
+    </row>
+    <row r="763" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G763" s="51"/>
+    </row>
+    <row r="764" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G764" s="51"/>
+    </row>
+    <row r="765" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G765" s="51"/>
+    </row>
+    <row r="766" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G766" s="51"/>
+    </row>
+    <row r="767" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G767" s="51"/>
+    </row>
+    <row r="768" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G768" s="51"/>
+    </row>
+    <row r="769" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G769" s="51"/>
+    </row>
+    <row r="770" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G770" s="51"/>
+    </row>
+    <row r="771" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G771" s="51"/>
+    </row>
+    <row r="772" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G772" s="51"/>
+    </row>
+    <row r="773" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G773" s="51"/>
+    </row>
+    <row r="774" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G774" s="51"/>
+    </row>
+    <row r="775" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G775" s="51"/>
+    </row>
+    <row r="776" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G776" s="51"/>
+    </row>
+    <row r="777" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G777" s="51"/>
+    </row>
+    <row r="778" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G778" s="51"/>
+    </row>
+    <row r="779" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G779" s="51"/>
+    </row>
+    <row r="780" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G780" s="51"/>
+    </row>
+    <row r="781" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G781" s="51"/>
+    </row>
+    <row r="782" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G782" s="51"/>
+    </row>
+    <row r="783" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G783" s="51"/>
+    </row>
+    <row r="784" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G784" s="51"/>
+    </row>
+    <row r="785" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G785" s="51"/>
+    </row>
+    <row r="786" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G786" s="51"/>
+    </row>
+    <row r="787" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G787" s="51"/>
+    </row>
+    <row r="788" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G788" s="51"/>
+    </row>
+    <row r="789" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G789" s="51"/>
+    </row>
+    <row r="790" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G790" s="51"/>
+    </row>
+    <row r="791" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G791" s="51"/>
+    </row>
+    <row r="792" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G792" s="51"/>
+    </row>
+    <row r="793" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G793" s="51"/>
+    </row>
+    <row r="794" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G794" s="51"/>
+    </row>
+    <row r="795" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G795" s="51"/>
+    </row>
+    <row r="796" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G796" s="51"/>
+    </row>
+    <row r="797" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G797" s="51"/>
+    </row>
+    <row r="798" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G798" s="51"/>
+    </row>
+    <row r="799" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G799" s="51"/>
+    </row>
+    <row r="800" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G800" s="51"/>
+    </row>
+    <row r="801" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G801" s="51"/>
+    </row>
+    <row r="802" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G802" s="51"/>
+    </row>
+    <row r="803" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G803" s="51"/>
+    </row>
+    <row r="804" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G804" s="51"/>
+    </row>
+    <row r="805" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G805" s="51"/>
+    </row>
+    <row r="806" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G806" s="51"/>
+    </row>
+    <row r="807" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G807" s="51"/>
+    </row>
+    <row r="808" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G808" s="51"/>
+    </row>
+    <row r="809" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G809" s="51"/>
+    </row>
+    <row r="810" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G810" s="51"/>
+    </row>
+    <row r="811" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G811" s="51"/>
+    </row>
+    <row r="812" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G812" s="51"/>
+    </row>
+    <row r="813" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G813" s="51"/>
+    </row>
+    <row r="814" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G814" s="51"/>
+    </row>
+    <row r="815" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G815" s="51"/>
+    </row>
+    <row r="816" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G816" s="51"/>
+    </row>
+    <row r="817" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G817" s="51"/>
+    </row>
+    <row r="818" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G818" s="51"/>
+    </row>
+    <row r="819" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G819" s="51"/>
+    </row>
+    <row r="820" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G820" s="51"/>
+    </row>
+    <row r="821" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G821" s="51"/>
+    </row>
+    <row r="822" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G822" s="51"/>
+    </row>
+    <row r="823" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G823" s="51"/>
+    </row>
+    <row r="824" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G824" s="51"/>
+    </row>
+    <row r="825" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G825" s="51"/>
+    </row>
+    <row r="826" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G826" s="51"/>
+    </row>
+    <row r="827" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G827" s="51"/>
+    </row>
+    <row r="828" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G828" s="51"/>
+    </row>
+    <row r="829" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G829" s="51"/>
+    </row>
+    <row r="830" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G830" s="51"/>
+    </row>
+    <row r="831" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G831" s="51"/>
+    </row>
+    <row r="832" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G832" s="51"/>
+    </row>
+    <row r="833" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G833" s="51"/>
+    </row>
+    <row r="834" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G834" s="51"/>
+    </row>
+    <row r="835" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G835" s="51"/>
+    </row>
+    <row r="836" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G836" s="51"/>
+    </row>
+    <row r="837" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G837" s="51"/>
+    </row>
+    <row r="838" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G838" s="51"/>
+    </row>
+    <row r="839" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G839" s="51"/>
+    </row>
+    <row r="840" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G840" s="51"/>
+    </row>
+    <row r="841" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G841" s="51"/>
+    </row>
+    <row r="842" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G842" s="51"/>
+    </row>
+    <row r="843" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G843" s="51"/>
+    </row>
+    <row r="844" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G844" s="51"/>
+    </row>
+    <row r="845" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G845" s="51"/>
+    </row>
+    <row r="846" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G846" s="51"/>
+    </row>
+    <row r="847" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G847" s="51"/>
+    </row>
+    <row r="848" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G848" s="51"/>
+    </row>
+    <row r="849" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G849" s="51"/>
+    </row>
+    <row r="850" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G850" s="51"/>
+    </row>
+    <row r="851" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G851" s="51"/>
+    </row>
+    <row r="852" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G852" s="51"/>
+    </row>
+    <row r="853" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G853" s="51"/>
+    </row>
+    <row r="854" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G854" s="51"/>
+    </row>
+    <row r="855" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G855" s="51"/>
+    </row>
+    <row r="856" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G856" s="51"/>
+    </row>
+    <row r="857" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G857" s="51"/>
+    </row>
+    <row r="858" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G858" s="51"/>
+    </row>
+    <row r="859" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G859" s="51"/>
+    </row>
+    <row r="860" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G860" s="51"/>
+    </row>
+    <row r="861" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G861" s="51"/>
+    </row>
+    <row r="862" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G862" s="51"/>
+    </row>
+    <row r="863" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G863" s="51"/>
+    </row>
+    <row r="864" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G864" s="51"/>
+    </row>
+    <row r="865" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G865" s="51"/>
+    </row>
+    <row r="866" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G866" s="51"/>
+    </row>
+    <row r="867" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G867" s="51"/>
+    </row>
+    <row r="868" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G868" s="51"/>
+    </row>
+    <row r="869" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G869" s="51"/>
+    </row>
+    <row r="870" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G870" s="51"/>
+    </row>
+    <row r="871" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G871" s="51"/>
+    </row>
+    <row r="872" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G872" s="51"/>
+    </row>
+    <row r="873" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G873" s="51"/>
+    </row>
+    <row r="874" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G874" s="51"/>
+    </row>
+    <row r="875" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G875" s="51"/>
+    </row>
+    <row r="876" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G876" s="51"/>
+    </row>
+    <row r="877" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G877" s="51"/>
+    </row>
+    <row r="878" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G878" s="51"/>
+    </row>
+    <row r="879" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G879" s="51"/>
+    </row>
+    <row r="880" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G880" s="51"/>
+    </row>
+    <row r="881" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G881" s="51"/>
+    </row>
+    <row r="882" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G882" s="51"/>
+    </row>
+    <row r="883" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G883" s="51"/>
+    </row>
+    <row r="884" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G884" s="51"/>
+    </row>
+    <row r="885" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G885" s="51"/>
+    </row>
+    <row r="886" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G886" s="51"/>
+    </row>
+    <row r="887" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G887" s="51"/>
+    </row>
+    <row r="888" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G888" s="51"/>
+    </row>
+    <row r="889" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G889" s="51"/>
+    </row>
+    <row r="890" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G890" s="51"/>
+    </row>
+    <row r="891" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G891" s="51"/>
+    </row>
+    <row r="892" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G892" s="51"/>
+    </row>
+    <row r="893" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G893" s="51"/>
+    </row>
+    <row r="894" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G894" s="51"/>
+    </row>
+    <row r="895" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G895" s="51"/>
+    </row>
+    <row r="896" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G896" s="51"/>
+    </row>
+    <row r="897" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G897" s="51"/>
+    </row>
+    <row r="898" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G898" s="51"/>
+    </row>
+    <row r="899" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G899" s="51"/>
+    </row>
+    <row r="900" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G900" s="51"/>
+    </row>
+    <row r="901" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G901" s="51"/>
+    </row>
+    <row r="902" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G902" s="51"/>
+    </row>
+    <row r="903" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G903" s="51"/>
+    </row>
+    <row r="904" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G904" s="51"/>
+    </row>
+    <row r="905" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G905" s="51"/>
+    </row>
+    <row r="906" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G906" s="51"/>
+    </row>
+    <row r="907" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G907" s="51"/>
+    </row>
+    <row r="908" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G908" s="51"/>
+    </row>
+    <row r="909" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G909" s="51"/>
+    </row>
+    <row r="910" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G910" s="51"/>
+    </row>
+    <row r="911" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G911" s="51"/>
+    </row>
+    <row r="912" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G912" s="51"/>
+    </row>
+    <row r="913" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G913" s="51"/>
+    </row>
+    <row r="914" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G914" s="51"/>
+    </row>
+    <row r="915" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G915" s="51"/>
+    </row>
+    <row r="916" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G916" s="51"/>
+    </row>
+    <row r="917" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G917" s="51"/>
+    </row>
+    <row r="918" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G918" s="51"/>
+    </row>
+    <row r="919" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G919" s="51"/>
+    </row>
+    <row r="920" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G920" s="51"/>
+    </row>
+    <row r="921" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G921" s="51"/>
+    </row>
+    <row r="922" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G922" s="51"/>
+    </row>
+    <row r="923" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G923" s="51"/>
+    </row>
+    <row r="924" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G924" s="51"/>
+    </row>
+    <row r="925" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G925" s="51"/>
+    </row>
+    <row r="926" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G926" s="51"/>
+    </row>
+    <row r="927" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G927" s="51"/>
+    </row>
+    <row r="928" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G928" s="51"/>
+    </row>
+    <row r="929" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G929" s="51"/>
+    </row>
+    <row r="930" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G930" s="51"/>
+    </row>
+    <row r="931" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G931" s="51"/>
+    </row>
+    <row r="932" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G932" s="51"/>
+    </row>
+    <row r="933" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G933" s="51"/>
+    </row>
+    <row r="934" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G934" s="51"/>
+    </row>
+    <row r="935" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G935" s="51"/>
+    </row>
+    <row r="936" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G936" s="51"/>
+    </row>
+    <row r="937" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G937" s="51"/>
+    </row>
+    <row r="938" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G938" s="51"/>
+    </row>
+    <row r="939" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G939" s="51"/>
+    </row>
+    <row r="940" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G940" s="51"/>
+    </row>
+    <row r="941" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G941" s="51"/>
+    </row>
+    <row r="942" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G942" s="51"/>
+    </row>
+    <row r="943" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G943" s="51"/>
+    </row>
+    <row r="944" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G944" s="51"/>
+    </row>
+    <row r="945" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G945" s="51"/>
+    </row>
+    <row r="946" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G946" s="51"/>
+    </row>
+    <row r="947" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G947" s="51"/>
+    </row>
+    <row r="948" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G948" s="51"/>
+    </row>
+    <row r="949" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G949" s="51"/>
+    </row>
+    <row r="950" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G950" s="51"/>
+    </row>
+    <row r="951" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G951" s="51"/>
+    </row>
+    <row r="952" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G952" s="51"/>
+    </row>
+    <row r="953" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G953" s="51"/>
+    </row>
+    <row r="954" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G954" s="51"/>
+    </row>
+    <row r="955" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G955" s="51"/>
+    </row>
+    <row r="956" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G956" s="51"/>
+    </row>
+    <row r="957" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G957" s="51"/>
+    </row>
+    <row r="958" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G958" s="51"/>
+    </row>
+    <row r="959" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G959" s="51"/>
+    </row>
+    <row r="960" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G960" s="51"/>
+    </row>
+    <row r="961" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G961" s="51"/>
+    </row>
+    <row r="962" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G962" s="51"/>
+    </row>
+    <row r="963" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G963" s="51"/>
+    </row>
+    <row r="964" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G964" s="51"/>
+    </row>
+    <row r="965" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G965" s="51"/>
+    </row>
+    <row r="966" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G966" s="51"/>
+    </row>
+    <row r="967" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G967" s="51"/>
+    </row>
+    <row r="968" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G968" s="51"/>
+    </row>
+    <row r="969" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G969" s="51"/>
+    </row>
+    <row r="970" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G970" s="51"/>
+    </row>
+    <row r="971" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G971" s="51"/>
+    </row>
+    <row r="972" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G972" s="51"/>
+    </row>
+    <row r="973" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G973" s="51"/>
+    </row>
+    <row r="974" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G974" s="51"/>
+    </row>
+    <row r="975" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G975" s="51"/>
+    </row>
+    <row r="976" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G976" s="51"/>
+    </row>
+    <row r="977" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G977" s="51"/>
+    </row>
+    <row r="978" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G978" s="51"/>
+    </row>
+    <row r="979" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G979" s="51"/>
+    </row>
+    <row r="980" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G980" s="51"/>
+    </row>
+    <row r="981" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G981" s="51"/>
+    </row>
+    <row r="982" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G982" s="51"/>
+    </row>
+    <row r="983" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G983" s="51"/>
+    </row>
+    <row r="984" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G984" s="51"/>
+    </row>
+    <row r="985" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G985" s="51"/>
+    </row>
+    <row r="986" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G986" s="51"/>
+    </row>
+    <row r="987" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G987" s="51"/>
+    </row>
+    <row r="988" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G988" s="51"/>
+    </row>
+    <row r="989" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G989" s="51"/>
+    </row>
+    <row r="990" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G990" s="51"/>
+    </row>
+    <row r="991" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G991" s="51"/>
+    </row>
+    <row r="992" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G992" s="51"/>
+    </row>
+    <row r="993" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G993" s="51"/>
+    </row>
+    <row r="994" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G994" s="51"/>
+    </row>
+    <row r="995" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G995" s="51"/>
+    </row>
+    <row r="996" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G996" s="51"/>
+    </row>
+    <row r="997" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G997" s="51"/>
+    </row>
+    <row r="998" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G998" s="51"/>
+    </row>
+    <row r="999" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G999" s="51"/>
+    </row>
+    <row r="1000" spans="7:7" ht="15.75" customHeight="1">
+      <c r="G1000" s="51"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>

</xml_diff>

<commit_message>
small fix: flanking for anderson promoter and updating to pSB1C5, and fixing form validation.
</commit_message>
<xml_diff>
--- a/Anderson Promoters/Anderson Promoters.xlsx
+++ b/Anderson Promoters/Anderson Promoters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakebeal/projects/BioTools/iGEM_distribution/Anderson Promoters/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinoo/_dev/distribution/iGEM-distribution/Anderson Promoters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A74BD0E7-87A3-C240-8973-1C92FA63FF17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2BEEDFD-EAFC-4C45-8868-C7D0221A43D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1780" yWindow="1300" windowWidth="34060" windowHeight="19800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30300" yWindow="-420" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts and Devices" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7666" uniqueCount="7547">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7684" uniqueCount="7553">
   <si>
     <t>Collection Name</t>
   </si>
@@ -22670,6 +22670,24 @@
   </si>
   <si>
     <t>1.0a2</t>
+  </si>
+  <si>
+    <t>pSB1C5</t>
+  </si>
+  <si>
+    <t>D1001</t>
+  </si>
+  <si>
+    <t>Includes BsaI and fusion site</t>
+  </si>
+  <si>
+    <t>L0 Promoter 5' Flanking Region</t>
+  </si>
+  <si>
+    <t>D1002</t>
+  </si>
+  <si>
+    <t>L0 Promoter 3' Flanking Region</t>
   </si>
 </sst>
 </file>
@@ -23491,8 +23509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M983"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -24293,17 +24311,17 @@
     </row>
     <row r="35" spans="1:13" ht="15.75" customHeight="1">
       <c r="A35" s="37" t="s">
-        <v>70</v>
+        <v>7547</v>
       </c>
       <c r="B35" s="37" t="s">
-        <v>71</v>
+        <v>4506</v>
       </c>
       <c r="D35" s="15"/>
       <c r="F35" t="s">
-        <v>11</v>
+        <v>7543</v>
       </c>
       <c r="G35" s="37" t="s">
-        <v>70</v>
+        <v>7547</v>
       </c>
       <c r="I35" t="s">
         <v>12</v>
@@ -24319,25 +24337,67 @@
       </c>
     </row>
     <row r="36" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A36" s="37"/>
-      <c r="B36" s="37"/>
+      <c r="A36" s="37" t="s">
+        <v>7548</v>
+      </c>
+      <c r="B36" s="37" t="s">
+        <v>1387</v>
+      </c>
+      <c r="C36" s="34" t="s">
+        <v>7549</v>
+      </c>
       <c r="D36" s="15"/>
-      <c r="G36" s="15"/>
-      <c r="I36"/>
+      <c r="E36" s="34" t="s">
+        <v>7550</v>
+      </c>
+      <c r="F36" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="G36" s="15" t="s">
+        <v>7548</v>
+      </c>
+      <c r="H36" s="34" t="s">
+        <v>7453</v>
+      </c>
+      <c r="I36" t="s">
+        <v>12</v>
+      </c>
       <c r="J36" t="b">
         <v>0</v>
       </c>
       <c r="K36" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L36" s="12">
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A37" s="37"/>
+      <c r="A37" s="37" t="s">
+        <v>7551</v>
+      </c>
+      <c r="B37" s="34" t="s">
+        <v>1387</v>
+      </c>
+      <c r="C37" s="34" t="s">
+        <v>7549</v>
+      </c>
       <c r="D37" s="15"/>
-      <c r="G37" s="15"/>
+      <c r="E37" s="34" t="s">
+        <v>7552</v>
+      </c>
+      <c r="F37" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="G37" s="15" t="s">
+        <v>7551</v>
+      </c>
+      <c r="H37" s="34" t="s">
+        <v>7453</v>
+      </c>
+      <c r="I37" s="34" t="s">
+        <v>12</v>
+      </c>
       <c r="J37" t="b">
         <v>0</v>
       </c>
@@ -25316,6 +25376,36 @@
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7AB12585-E89C-D848-BD86-057931EA1209}">
+          <x14:formula1>
+            <xm:f>'Ontology Terms'!$B$2:$B$2518</xm:f>
+          </x14:formula1>
+          <xm:sqref>B15:B38</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{39ADB128-EE1A-3D47-86C5-630A7E0BEDE3}">
+          <x14:formula1>
+            <xm:f>data_source!$B$2:$B$11</xm:f>
+          </x14:formula1>
+          <xm:sqref>F15:F38</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C1A95308-6EB6-B147-9283-589A0E7C9EE2}">
+          <x14:formula1>
+            <xm:f>'Ontology Terms'!$F$2:$F$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>J15:K38</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{83F6E5C9-8372-5549-A791-78C4EEF88B98}">
+          <x14:formula1>
+            <xm:f>'Organism Terms'!$A$2:$A$44</xm:f>
+          </x14:formula1>
+          <xm:sqref>H15:I38</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -25323,8 +25413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -25643,12 +25733,17 @@
         <v>1</v>
       </c>
       <c r="E14" s="37" t="s">
-        <v>70</v>
-      </c>
-      <c r="G14" s="37" t="s">
+        <v>7547</v>
+      </c>
+      <c r="G14" s="34" t="s">
+        <v>7548</v>
+      </c>
+      <c r="H14" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="I14" s="26"/>
+      <c r="I14" s="26" t="s">
+        <v>7551</v>
+      </c>
     </row>
     <row r="15" spans="1:26" ht="16" customHeight="1">
       <c r="D15" t="b">
@@ -25690,6 +25785,18 @@
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CDEF37BD-5F5A-5048-8460-61ED8EE37430}">
+          <x14:formula1>
+            <xm:f>'Ontology Terms'!$F$2:$F$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>D14:D20</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
test for adding flanking sequences for extra bases
</commit_message>
<xml_diff>
--- a/Anderson Promoters/Anderson Promoters.xlsx
+++ b/Anderson Promoters/Anderson Promoters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinoo/_dev/distribution/iGEM-distribution/Anderson Promoters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2BEEDFD-EAFC-4C45-8868-C7D0221A43D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5655923E-B1A9-9143-A3BA-E22FA625C11B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30300" yWindow="-420" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7684" uniqueCount="7553">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7700" uniqueCount="7556">
   <si>
     <t>Collection Name</t>
   </si>
@@ -22688,6 +22688,15 @@
   </si>
   <si>
     <t>L0 Promoter 3' Flanking Region</t>
+  </si>
+  <si>
+    <t>D2001</t>
+  </si>
+  <si>
+    <t>Extra nonsense bases for synthesis</t>
+  </si>
+  <si>
+    <t>D2002</t>
   </si>
 </sst>
 </file>
@@ -23266,7 +23275,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A14:M38" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A14:M40" headerRowCount="0">
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2"/>
@@ -23509,8 +23518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M983"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -24409,9 +24418,28 @@
       </c>
     </row>
     <row r="38" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A38" s="37"/>
+      <c r="A38" s="37" t="s">
+        <v>7553</v>
+      </c>
+      <c r="B38" s="34" t="s">
+        <v>1387</v>
+      </c>
+      <c r="C38" s="34" t="s">
+        <v>7554</v>
+      </c>
       <c r="D38" s="15"/>
-      <c r="G38" s="15"/>
+      <c r="F38" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="G38" s="15" t="s">
+        <v>7553</v>
+      </c>
+      <c r="H38" s="34" t="s">
+        <v>7453</v>
+      </c>
+      <c r="I38" s="34" t="s">
+        <v>12</v>
+      </c>
       <c r="J38" t="b">
         <v>0</v>
       </c>
@@ -24422,8 +24450,53 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="15.75" customHeight="1"/>
-    <row r="40" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="39" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A39" s="37" t="s">
+        <v>7555</v>
+      </c>
+      <c r="B39" s="34" t="s">
+        <v>1387</v>
+      </c>
+      <c r="C39" s="34" t="s">
+        <v>7554</v>
+      </c>
+      <c r="D39" s="15"/>
+      <c r="F39" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="G39" s="15" t="s">
+        <v>7555</v>
+      </c>
+      <c r="H39" s="34" t="s">
+        <v>7453</v>
+      </c>
+      <c r="I39" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="J39" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="K39" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="L39" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A40" s="37"/>
+      <c r="D40" s="15"/>
+      <c r="G40" s="15"/>
+      <c r="J40" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="K40" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="L40" s="12">
+        <v>2</v>
+      </c>
+    </row>
     <row r="41" spans="1:13" ht="15.75" customHeight="1"/>
     <row r="42" spans="1:13" ht="15.75" customHeight="1"/>
     <row r="43" spans="1:13" ht="15.75" customHeight="1"/>
@@ -25383,25 +25456,25 @@
           <x14:formula1>
             <xm:f>'Ontology Terms'!$B$2:$B$2518</xm:f>
           </x14:formula1>
-          <xm:sqref>B15:B38</xm:sqref>
+          <xm:sqref>B15:B40</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{39ADB128-EE1A-3D47-86C5-630A7E0BEDE3}">
           <x14:formula1>
             <xm:f>data_source!$B$2:$B$11</xm:f>
           </x14:formula1>
-          <xm:sqref>F15:F38</xm:sqref>
+          <xm:sqref>F15:F40</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C1A95308-6EB6-B147-9283-589A0E7C9EE2}">
           <x14:formula1>
             <xm:f>'Ontology Terms'!$F$2:$F$3</xm:f>
           </x14:formula1>
-          <xm:sqref>J15:K38</xm:sqref>
+          <xm:sqref>J15:K40</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{83F6E5C9-8372-5549-A791-78C4EEF88B98}">
           <x14:formula1>
             <xm:f>'Organism Terms'!$A$2:$A$44</xm:f>
           </x14:formula1>
-          <xm:sqref>H15:I38</xm:sqref>
+          <xm:sqref>H15:I40</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -25414,7 +25487,7 @@
   <dimension ref="A1:Z20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14:D20"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -25736,13 +25809,19 @@
         <v>7547</v>
       </c>
       <c r="G14" s="34" t="s">
+        <v>7553</v>
+      </c>
+      <c r="H14" s="37" t="s">
         <v>7548</v>
       </c>
-      <c r="H14" s="37" t="s">
+      <c r="I14" s="26" t="s">
         <v>109</v>
       </c>
-      <c r="I14" s="26" t="s">
+      <c r="J14" s="34" t="s">
         <v>7551</v>
+      </c>
+      <c r="K14" s="34" t="s">
+        <v>7555</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="16" customHeight="1">

</xml_diff>

<commit_message>
error that I think was do to explicit entry (accidental) into sequence length. removed!
</commit_message>
<xml_diff>
--- a/Anderson Promoters/Anderson Promoters.xlsx
+++ b/Anderson Promoters/Anderson Promoters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinoo/_dev/distribution/iGEM-distribution/Anderson Promoters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5655923E-B1A9-9143-A3BA-E22FA625C11B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B79E8C37-3DD8-1140-86B0-FD8996816282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30300" yWindow="-420" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23518,8 +23518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M983"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" topLeftCell="C11" workbookViewId="0">
+      <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -24480,22 +24480,14 @@
         <v>0</v>
       </c>
       <c r="L39" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="15.75" customHeight="1">
       <c r="A40" s="37"/>
       <c r="D40" s="15"/>
       <c r="G40" s="15"/>
-      <c r="J40" s="34" t="b">
-        <v>0</v>
-      </c>
-      <c r="K40" s="34" t="b">
-        <v>0</v>
-      </c>
-      <c r="L40" s="12">
-        <v>2</v>
-      </c>
+      <c r="L40" s="12"/>
     </row>
     <row r="41" spans="1:13" ht="15.75" customHeight="1"/>
     <row r="42" spans="1:13" ht="15.75" customHeight="1"/>
@@ -25486,7 +25478,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B2" workbookViewId="0">
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
- draft fix for anderson promoters, needs review - not all promoters that failed synthesis (unable to build) in pSB1C5 were able to be cloned into pSB1C3 (ex. J23103)
</commit_message>
<xml_diff>
--- a/Anderson Promoters/Anderson Promoters.xlsx
+++ b/Anderson Promoters/Anderson Promoters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinoo/_dev/distribution/iGEM-distribution/Anderson Promoters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D886A982-6459-A44C-95EB-93E9C6BDDA12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B118B0-60FF-8147-B229-D49B81B3E9DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30300" yWindow="-420" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts and Devices" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7695" uniqueCount="7555">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7714" uniqueCount="7559">
   <si>
     <t>Collection Name</t>
   </si>
@@ -22693,7 +22693,19 @@
     <t>D2002</t>
   </si>
   <si>
-    <t>J23100, J23101, J23102, J23103, J23104, J23105, J23106, J23107, J23108, J23109, J23110, J23111, J23113, J23114, J23115, J23116, J23117, J23118, J23119</t>
+    <t>J23101, J23103, J23104, J23106, J23107, J23108, J23111, J23113, J23115, J23117, J23118</t>
+  </si>
+  <si>
+    <t>Unable to build</t>
+  </si>
+  <si>
+    <t>J23100, J23102, J23105, J23109, J23110, J23114, J23116, J23119</t>
+  </si>
+  <si>
+    <t>Anderson Promoters in pSB1C3</t>
+  </si>
+  <si>
+    <t>J23101, J23104, J23106, J23107, J23111, J23113, J23115, J23117, J23118</t>
   </si>
 </sst>
 </file>
@@ -23516,7 +23528,7 @@
   <dimension ref="A1:M983"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -24471,9 +24483,28 @@
       </c>
     </row>
     <row r="40" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A40" s="37"/>
+      <c r="A40" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="B40" s="37" t="s">
+        <v>4504</v>
+      </c>
       <c r="D40" s="15"/>
-      <c r="G40" s="15"/>
+      <c r="F40" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="G40" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="I40" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="J40" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="K40" s="34" t="b">
+        <v>1</v>
+      </c>
       <c r="L40" s="12"/>
     </row>
     <row r="41" spans="1:13" ht="15.75" customHeight="1"/>
@@ -25465,8 +25496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -25794,7 +25825,7 @@
         <v>7546</v>
       </c>
       <c r="I14" s="26" t="s">
-        <v>7554</v>
+        <v>7556</v>
       </c>
       <c r="J14" s="34" t="s">
         <v>7549</v>
@@ -25804,16 +25835,56 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="16" customHeight="1">
+      <c r="A15" s="34" t="s">
+        <v>7557</v>
+      </c>
       <c r="D15" t="b">
-        <v>0</v>
-      </c>
-      <c r="K15" s="15"/>
+        <v>1</v>
+      </c>
+      <c r="E15" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="G15" s="34" t="s">
+        <v>7551</v>
+      </c>
+      <c r="H15" s="37" t="s">
+        <v>7546</v>
+      </c>
+      <c r="I15" s="26" t="s">
+        <v>7558</v>
+      </c>
+      <c r="J15" s="34" t="s">
+        <v>7549</v>
+      </c>
+      <c r="K15" s="34" t="s">
+        <v>7553</v>
+      </c>
     </row>
     <row r="16" spans="1:26" ht="15" customHeight="1">
+      <c r="A16" s="34" t="s">
+        <v>7555</v>
+      </c>
       <c r="D16" t="b">
         <v>0</v>
       </c>
-      <c r="I16" s="26"/>
+      <c r="E16" s="37" t="s">
+        <v>7545</v>
+      </c>
+      <c r="G16" s="34" t="s">
+        <v>7551</v>
+      </c>
+      <c r="H16" s="37" t="s">
+        <v>7546</v>
+      </c>
+      <c r="I16" s="26" t="s">
+        <v>7554</v>
+      </c>
+      <c r="J16" s="34" t="s">
+        <v>7549</v>
+      </c>
+      <c r="K16" s="34" t="s">
+        <v>7553</v>
+      </c>
     </row>
     <row r="17" spans="4:9" ht="15" customHeight="1">
       <c r="D17" t="b">

</xml_diff>

<commit_message>
Fix missing zero on sequence listing for pSB1C3
</commit_message>
<xml_diff>
--- a/Anderson Promoters/Anderson Promoters.xlsx
+++ b/Anderson Promoters/Anderson Promoters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinoo/_dev/distribution/iGEM-distribution/Anderson Promoters/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbeal/projects/BioTools/iGEM_distribution/Anderson Promoters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B118B0-60FF-8147-B229-D49B81B3E9DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A086853-F8B7-C045-A87C-AD5CA9C3457F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23527,8 +23527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M983"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -24505,7 +24505,9 @@
       <c r="K40" s="34" t="b">
         <v>1</v>
       </c>
-      <c r="L40" s="12"/>
+      <c r="L40" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="41" spans="1:13" ht="15.75" customHeight="1"/>
     <row r="42" spans="1:13" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Updated several collections with unable to be built and cloned into pSB1C3
List of unable to be built but also unable to be cloned from linear (for different reasons)
K1033902 (Chromoproteins)
BCD13 (RBS)
BBa_B0010 (Terminators)
J23103 / J23108 (Anderson Promoters)
</commit_message>
<xml_diff>
--- a/Anderson Promoters/Anderson Promoters.xlsx
+++ b/Anderson Promoters/Anderson Promoters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbeal/projects/BioTools/iGEM_distribution/Anderson Promoters/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinoo/_dev/distribution/iGEM-distribution/Anderson Promoters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A086853-F8B7-C045-A87C-AD5CA9C3457F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86B3D162-041B-A84D-B897-F05FA1D7CA2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts and Devices" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7714" uniqueCount="7559">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7716" uniqueCount="7561">
   <si>
     <t>Collection Name</t>
   </si>
@@ -22706,6 +22706,12 @@
   </si>
   <si>
     <t>J23101, J23104, J23106, J23107, J23111, J23113, J23115, J23117, J23118</t>
+  </si>
+  <si>
+    <t>Constructs belonged to original build plan, but unable to synthesize as clonal product by TWIST</t>
+  </si>
+  <si>
+    <t>Synthesized as linear fragments and cloned into pSB1C3</t>
   </si>
 </sst>
 </file>
@@ -23033,7 +23039,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -23085,6 +23091,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -23527,7 +23536,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M983"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
+    <sheetView topLeftCell="B5" workbookViewId="0">
       <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
@@ -25498,8 +25507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -25840,6 +25849,9 @@
       <c r="A15" s="34" t="s">
         <v>7557</v>
       </c>
+      <c r="B15" s="37" t="s">
+        <v>7560</v>
+      </c>
       <c r="D15" t="b">
         <v>1</v>
       </c>
@@ -25852,7 +25864,7 @@
       <c r="H15" s="37" t="s">
         <v>7546</v>
       </c>
-      <c r="I15" s="26" t="s">
+      <c r="I15" s="45" t="s">
         <v>7558</v>
       </c>
       <c r="J15" s="34" t="s">
@@ -25866,6 +25878,9 @@
       <c r="A16" s="34" t="s">
         <v>7555</v>
       </c>
+      <c r="B16" s="37" t="s">
+        <v>7559</v>
+      </c>
       <c r="D16" t="b">
         <v>0</v>
       </c>
@@ -25878,7 +25893,7 @@
       <c r="H16" s="37" t="s">
         <v>7546</v>
       </c>
-      <c r="I16" s="26" t="s">
+      <c r="I16" s="45" t="s">
         <v>7554</v>
       </c>
       <c r="J16" s="34" t="s">

</xml_diff>